<commit_message>
Summer & Fall 2019 updates
</commit_message>
<xml_diff>
--- a/schedule/semester/schedule.xlsx
+++ b/schedule/semester/schedule.xlsx
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8590" uniqueCount="1475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8490" uniqueCount="1505">
   <si>
     <t>ELECTRICAL AND COMPUTER ENGINEERING</t>
   </si>
@@ -3913,9 +3913,6 @@
     <t>Fall SEMESTER 2019 COURSE LIST</t>
   </si>
   <si>
-    <t xml:space="preserve"> SUMMER INTERSESSION 2019 COURSE LIST</t>
-  </si>
-  <si>
     <t xml:space="preserve"> SPRING SEMESTER 2019 COURSE LIST</t>
   </si>
   <si>
@@ -4369,9 +4366,6 @@
     <t>T 1000-1150AM</t>
   </si>
   <si>
-    <t>T 1200-150PM</t>
-  </si>
-  <si>
     <t>W 1000-1150AM</t>
   </si>
   <si>
@@ -4486,9 +4480,6 @@
     <t>Posted 1/28/2019</t>
   </si>
   <si>
-    <t>T 800-940AM</t>
-  </si>
-  <si>
     <t>November 25-27</t>
   </si>
   <si>
@@ -4505,6 +4496,105 @@
   </si>
   <si>
     <t>August 19                  </t>
+  </si>
+  <si>
+    <t>EE 4310-80</t>
+  </si>
+  <si>
+    <t>TR 12:30pm-4:45pm</t>
+  </si>
+  <si>
+    <t>Programming in Python</t>
+  </si>
+  <si>
+    <t>TR 8:00am-12:15pm</t>
+  </si>
+  <si>
+    <t>EE 5330-80</t>
+  </si>
+  <si>
+    <t>Computer Methods in Power Systems</t>
+  </si>
+  <si>
+    <t>TR 6:00pm-10:15pm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        SUMMER 2019 COURSE LIST (Session B: 5 WEEK SESSION, MAY 28 TO JULY 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        SUMMER 2019 COURSE LIST (Session C: 5 WEEK SESSION, JULY 8 TO AUGUST 10)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        SUMMER 2019 COURSE LIST (Session A: 10 WEEK SESSION, May 28 TO AUGUST 10)</t>
+  </si>
+  <si>
+    <t>EE 3000</t>
+  </si>
+  <si>
+    <t>Posted 2/21/2019</t>
+  </si>
+  <si>
+    <t>Posted 2/20/2019</t>
+  </si>
+  <si>
+    <t>SH264/SH260</t>
+  </si>
+  <si>
+    <t>F 150-420PM</t>
+  </si>
+  <si>
+    <t>W 150-420PM</t>
+  </si>
+  <si>
+    <t>T 1010AM-12PM</t>
+  </si>
+  <si>
+    <t>R 1055AM-125PM</t>
+  </si>
+  <si>
+    <t>F 1055AM-125PM</t>
+  </si>
+  <si>
+    <t>T 1210-200PM</t>
+  </si>
+  <si>
+    <t>R 150-420PM</t>
+  </si>
+  <si>
+    <t>ENGR3010-01</t>
+  </si>
+  <si>
+    <t>ENGR3010-02</t>
+  </si>
+  <si>
+    <t>ENGR3010-03</t>
+  </si>
+  <si>
+    <t>KHB2015</t>
+  </si>
+  <si>
+    <t>T 210-400PM</t>
+  </si>
+  <si>
+    <t>TR 210-300PM</t>
+  </si>
+  <si>
+    <t>KHC4077</t>
+  </si>
+  <si>
+    <t>ETC251/ETC252</t>
+  </si>
+  <si>
+    <t>ETA309</t>
+  </si>
+  <si>
+    <t>KHC4071</t>
+  </si>
+  <si>
+    <t>KHC2094</t>
+  </si>
+  <si>
+    <t>F 200-340PM</t>
   </si>
 </sst>
 </file>
@@ -7738,17 +7828,17 @@
       </c>
       <c r="E1" s="418"/>
       <c r="F1" s="458" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="410" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="409"/>
       <c r="C2" s="409"/>
       <c r="D2" s="449" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="E2" s="449" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="F2" s="458"/>
     </row>
@@ -7759,7 +7849,7 @@
         <v>1110</v>
       </c>
       <c r="E3" s="449" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="F3" s="449"/>
     </row>
@@ -7770,10 +7860,10 @@
       <c r="B4" s="457"/>
       <c r="C4" s="457"/>
       <c r="D4" s="449" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="E4" s="449" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="F4" s="449"/>
     </row>
@@ -7887,7 +7977,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="410" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="407" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="B1" s="408"/>
       <c r="C1" s="409"/>
@@ -7896,7 +7986,7 @@
       </c>
       <c r="E1" s="418"/>
       <c r="F1" s="458" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="410" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
@@ -8003,19 +8093,19 @@
     </row>
     <row r="13" spans="1:6" ht="12" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="413" t="s">
+        <v>1354</v>
+      </c>
+      <c r="B13" s="412" t="s">
         <v>1355</v>
-      </c>
-      <c r="B13" s="412" t="s">
-        <v>1356</v>
       </c>
       <c r="C13" s="414">
         <v>3</v>
       </c>
       <c r="D13" s="412" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="E13" s="412" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="F13" s="412" t="s">
         <v>119</v>
@@ -8023,10 +8113,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="413" t="s">
+        <v>1349</v>
+      </c>
+      <c r="B14" s="412" t="s">
         <v>1350</v>
-      </c>
-      <c r="B14" s="412" t="s">
-        <v>1351</v>
       </c>
       <c r="C14" s="414">
         <v>3</v>
@@ -8035,7 +8125,7 @@
         <v>64</v>
       </c>
       <c r="E14" s="412" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="F14" s="412" t="s">
         <v>89</v>
@@ -8043,7 +8133,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="413" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="B15" s="412" t="s">
         <v>801</v>
@@ -8055,7 +8145,7 @@
         <v>45</v>
       </c>
       <c r="E15" s="412" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="F15" s="412" t="s">
         <v>89</v>
@@ -8111,7 +8201,7 @@
       </c>
       <c r="E1" s="418"/>
       <c r="F1" s="458" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="410" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
@@ -9257,7 +9347,7 @@
         <v>1031</v>
       </c>
       <c r="D63" s="412" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="E63" s="412" t="s">
         <v>942</v>
@@ -9397,7 +9487,7 @@
         <v>3</v>
       </c>
       <c r="D70" s="412" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="E70" s="412" t="s">
         <v>964</v>
@@ -9616,7 +9706,7 @@
       </c>
       <c r="E1" s="418"/>
       <c r="F1" s="458" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="410" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
@@ -11148,7 +11238,7 @@
       </c>
       <c r="E1" s="418"/>
       <c r="F1" s="458" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="410" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
@@ -11537,7 +11627,7 @@
       </c>
       <c r="E1" s="418"/>
       <c r="F1" s="458" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="410" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
@@ -18931,17 +19021,17 @@
       </c>
       <c r="E1" s="418"/>
       <c r="F1" s="458" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="410" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="409"/>
       <c r="C2" s="409"/>
       <c r="D2" s="449" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="E2" s="449" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="F2" s="458"/>
     </row>
@@ -18949,7 +19039,7 @@
       <c r="B3" s="409"/>
       <c r="C3" s="409"/>
       <c r="D3" s="449" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="E3" s="449" t="s">
         <v>1136</v>
@@ -18963,10 +19053,10 @@
       <c r="B4" s="459"/>
       <c r="C4" s="459"/>
       <c r="D4" s="449" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="E4" s="449" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="F4" s="449"/>
     </row>
@@ -18975,10 +19065,10 @@
       <c r="B5" s="459"/>
       <c r="C5" s="459"/>
       <c r="D5" s="449" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="E5" s="449" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="410" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
@@ -18986,7 +19076,7 @@
       <c r="B6" s="459"/>
       <c r="C6" s="459"/>
       <c r="D6" s="449" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="E6" s="449" t="s">
         <v>1230</v>
@@ -19000,10 +19090,10 @@
       <c r="B7" s="460"/>
       <c r="C7" s="460"/>
       <c r="D7" s="449" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="E7" s="449" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="F7" s="449"/>
     </row>
@@ -19012,7 +19102,7 @@
       <c r="B8" s="460"/>
       <c r="C8" s="460"/>
       <c r="D8" s="449" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="E8" s="449" t="s">
         <v>1102</v>
@@ -19026,7 +19116,7 @@
         <v>1141</v>
       </c>
       <c r="E9" s="449" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="410" customFormat="1" ht="9" x14ac:dyDescent="0.15">
@@ -27987,13 +28077,13 @@
   <sheetPr codeName="Sheet43">
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:F82"/>
+  <dimension ref="A1:F77"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" ySplit="12" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -28009,7 +28099,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="410" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="407" t="s">
-        <v>1113</v>
+        <v>1484</v>
       </c>
       <c r="B1" s="408"/>
       <c r="C1" s="409"/>
@@ -28018,17 +28108,17 @@
       </c>
       <c r="E1" s="418"/>
       <c r="F1" s="458" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="410" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="409"/>
       <c r="C2" s="409"/>
       <c r="D2" s="449" t="s">
-        <v>1474</v>
+        <v>1471</v>
       </c>
       <c r="E2" s="449" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="F2" s="458"/>
     </row>
@@ -28036,7 +28126,7 @@
       <c r="B3" s="409"/>
       <c r="C3" s="409"/>
       <c r="D3" s="406" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="E3" s="449" t="s">
         <v>1227</v>
@@ -28050,7 +28140,7 @@
       <c r="B4" s="457"/>
       <c r="C4" s="457"/>
       <c r="D4" s="449" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="E4" s="449" t="s">
         <v>1228</v>
@@ -28074,10 +28164,10 @@
       <c r="B6" s="457"/>
       <c r="C6" s="457"/>
       <c r="D6" s="449" t="s">
-        <v>1469</v>
+        <v>1466</v>
       </c>
       <c r="E6" s="449" t="s">
-        <v>1471</v>
+        <v>1468</v>
       </c>
       <c r="F6" s="451"/>
     </row>
@@ -28088,7 +28178,7 @@
       <c r="B7" s="457"/>
       <c r="C7" s="457"/>
       <c r="D7" s="449" t="s">
-        <v>1470</v>
+        <v>1467</v>
       </c>
       <c r="E7" s="449" t="s">
         <v>1231</v>
@@ -28100,7 +28190,7 @@
       <c r="B8" s="457"/>
       <c r="C8" s="457"/>
       <c r="D8" s="449" t="s">
-        <v>1472</v>
+        <v>1469</v>
       </c>
       <c r="E8" s="449" t="s">
         <v>1101</v>
@@ -28112,10 +28202,10 @@
       <c r="B9" s="457"/>
       <c r="C9" s="457"/>
       <c r="D9" s="406" t="s">
-        <v>1473</v>
+        <v>1470</v>
       </c>
       <c r="E9" s="449" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="F9" s="451"/>
     </row>
@@ -28158,7 +28248,7 @@
         <v>1001</v>
       </c>
       <c r="B13" s="412" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="C13" s="414">
         <v>3</v>
@@ -28170,7 +28260,7 @@
         <v>931</v>
       </c>
       <c r="F13" s="412" t="s">
-        <v>1387</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -28184,7 +28274,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="412" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="F14" s="412" t="s">
         <v>14</v>
@@ -28234,11 +28324,14 @@
       <c r="C17" s="414">
         <v>2</v>
       </c>
+      <c r="D17" s="412" t="s">
+        <v>481</v>
+      </c>
       <c r="E17" s="412" t="s">
-        <v>1388</v>
+        <v>1425</v>
       </c>
       <c r="F17" s="412" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -28251,11 +28344,14 @@
       <c r="C18" s="414">
         <v>1</v>
       </c>
+      <c r="D18" s="412" t="s">
+        <v>481</v>
+      </c>
       <c r="E18" s="412" t="s">
-        <v>1329</v>
+        <v>1486</v>
       </c>
       <c r="F18" s="412" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -28268,11 +28364,14 @@
       <c r="C19" s="414">
         <v>2</v>
       </c>
+      <c r="D19" s="412" t="s">
+        <v>481</v>
+      </c>
       <c r="E19" s="412" t="s">
-        <v>1330</v>
+        <v>1426</v>
       </c>
       <c r="F19" s="412" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -28285,11 +28384,14 @@
       <c r="C20" s="414">
         <v>1</v>
       </c>
+      <c r="D20" s="412" t="s">
+        <v>481</v>
+      </c>
       <c r="E20" s="412" t="s">
-        <v>1210</v>
+        <v>1487</v>
       </c>
       <c r="F20" s="412" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -28302,14 +28404,11 @@
       <c r="C21" s="414">
         <v>2</v>
       </c>
-      <c r="D21" s="412" t="s">
-        <v>59</v>
-      </c>
       <c r="E21" s="412" t="s">
-        <v>1062</v>
+        <v>1488</v>
       </c>
       <c r="F21" s="412" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -28322,14 +28421,11 @@
       <c r="C22" s="414">
         <v>1</v>
       </c>
-      <c r="D22" s="412" t="s">
-        <v>59</v>
-      </c>
       <c r="E22" s="412" t="s">
-        <v>938</v>
+        <v>1489</v>
       </c>
       <c r="F22" s="412" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -28342,9 +28438,6 @@
       <c r="C23" s="414">
         <v>1</v>
       </c>
-      <c r="D23" s="412" t="s">
-        <v>741</v>
-      </c>
       <c r="E23" s="412" t="s">
         <v>919</v>
       </c>
@@ -28362,9 +28455,6 @@
       <c r="C24" s="414">
         <v>1</v>
       </c>
-      <c r="D24" s="412" t="s">
-        <v>1366</v>
-      </c>
       <c r="E24" s="412" t="s">
         <v>936</v>
       </c>
@@ -28382,9 +28472,6 @@
       <c r="C25" s="414">
         <v>1</v>
       </c>
-      <c r="D25" s="412" t="s">
-        <v>1366</v>
-      </c>
       <c r="E25" s="412" t="s">
         <v>1034</v>
       </c>
@@ -28402,8 +28489,11 @@
       <c r="C26" s="414">
         <v>2</v>
       </c>
+      <c r="D26" s="412" t="s">
+        <v>481</v>
+      </c>
       <c r="E26" s="412" t="s">
-        <v>1389</v>
+        <v>1428</v>
       </c>
       <c r="F26" s="412" t="s">
         <v>100</v>
@@ -28419,8 +28509,11 @@
       <c r="C27" s="414">
         <v>1</v>
       </c>
+      <c r="D27" s="412" t="s">
+        <v>481</v>
+      </c>
       <c r="E27" s="412" t="s">
-        <v>1331</v>
+        <v>1490</v>
       </c>
       <c r="F27" s="412" t="s">
         <v>100</v>
@@ -28436,11 +28529,8 @@
       <c r="C28" s="414">
         <v>2</v>
       </c>
-      <c r="D28" s="412" t="s">
-        <v>743</v>
-      </c>
       <c r="E28" s="412" t="s">
-        <v>1468</v>
+        <v>1378</v>
       </c>
       <c r="F28" s="412" t="s">
         <v>100</v>
@@ -28456,9 +28546,6 @@
       <c r="C29" s="414">
         <v>1</v>
       </c>
-      <c r="D29" s="412" t="s">
-        <v>743</v>
-      </c>
       <c r="E29" s="412" t="s">
         <v>1171</v>
       </c>
@@ -28476,11 +28563,8 @@
       <c r="C30" s="414">
         <v>2</v>
       </c>
-      <c r="D30" s="412" t="s">
-        <v>811</v>
-      </c>
       <c r="E30" s="412" t="s">
-        <v>1390</v>
+        <v>1491</v>
       </c>
       <c r="F30" s="412" t="s">
         <v>100</v>
@@ -28496,11 +28580,8 @@
       <c r="C31" s="414">
         <v>1</v>
       </c>
-      <c r="D31" s="412" t="s">
-        <v>811</v>
-      </c>
       <c r="E31" s="412" t="s">
-        <v>1333</v>
+        <v>1492</v>
       </c>
       <c r="F31" s="412" t="s">
         <v>100</v>
@@ -28508,130 +28589,118 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="413" t="s">
-        <v>1359</v>
+        <v>1006</v>
       </c>
       <c r="B32" s="412" t="s">
-        <v>921</v>
+        <v>1178</v>
       </c>
       <c r="C32" s="414">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D32" s="412" t="s">
-        <v>741</v>
+        <v>912</v>
       </c>
       <c r="E32" s="412" t="s">
-        <v>1360</v>
+        <v>924</v>
       </c>
       <c r="F32" s="412" t="s">
-        <v>100</v>
+        <v>432</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="413" t="s">
-        <v>1361</v>
+        <v>1007</v>
       </c>
       <c r="B33" s="412" t="s">
-        <v>921</v>
+        <v>925</v>
       </c>
       <c r="C33" s="414">
         <v>1</v>
       </c>
-      <c r="D33" s="412" t="s">
-        <v>741</v>
-      </c>
       <c r="E33" s="412" t="s">
-        <v>1362</v>
+        <v>926</v>
       </c>
       <c r="F33" s="412" t="s">
-        <v>100</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="413" t="s">
-        <v>1391</v>
+        <v>1493</v>
       </c>
       <c r="B34" s="412" t="s">
-        <v>1392</v>
+        <v>927</v>
       </c>
       <c r="C34" s="414">
         <v>3</v>
       </c>
-      <c r="D34" s="412" t="s">
-        <v>1393</v>
-      </c>
       <c r="E34" s="412" t="s">
-        <v>929</v>
+        <v>950</v>
       </c>
       <c r="F34" s="412" t="s">
-        <v>1394</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="413" t="s">
-        <v>1006</v>
+        <v>1494</v>
       </c>
       <c r="B35" s="412" t="s">
-        <v>1178</v>
+        <v>927</v>
       </c>
       <c r="C35" s="414">
         <v>3</v>
       </c>
-      <c r="D35" s="412" t="s">
-        <v>912</v>
-      </c>
       <c r="E35" s="412" t="s">
-        <v>924</v>
+        <v>947</v>
       </c>
       <c r="F35" s="412" t="s">
-        <v>432</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="413" t="s">
-        <v>1007</v>
+        <v>1495</v>
       </c>
       <c r="B36" s="412" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="C36" s="414">
-        <v>1</v>
-      </c>
-      <c r="D36" s="412" t="s">
-        <v>1219</v>
+        <v>3</v>
       </c>
       <c r="E36" s="412" t="s">
-        <v>926</v>
+        <v>972</v>
       </c>
       <c r="F36" s="412" t="s">
-        <v>66</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="413" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="B37" s="412" t="s">
-        <v>927</v>
+        <v>1179</v>
       </c>
       <c r="C37" s="414">
         <v>3</v>
       </c>
       <c r="D37" s="412" t="s">
-        <v>1363</v>
+        <v>34</v>
       </c>
       <c r="E37" s="412" t="s">
-        <v>972</v>
+        <v>929</v>
       </c>
       <c r="F37" s="412" t="s">
-        <v>1334</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="413" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="B38" s="412" t="s">
-        <v>1179</v>
+        <v>1414</v>
       </c>
       <c r="C38" s="414">
         <v>3</v>
@@ -28640,18 +28709,18 @@
         <v>34</v>
       </c>
       <c r="E38" s="412" t="s">
-        <v>929</v>
+        <v>914</v>
       </c>
       <c r="F38" s="412" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="413" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="B39" s="412" t="s">
-        <v>1415</v>
+        <v>979</v>
       </c>
       <c r="C39" s="414">
         <v>3</v>
@@ -28660,55 +28729,52 @@
         <v>34</v>
       </c>
       <c r="E39" s="412" t="s">
-        <v>914</v>
+        <v>938</v>
       </c>
       <c r="F39" s="412" t="s">
-        <v>1387</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="413" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="B40" s="412" t="s">
-        <v>979</v>
+        <v>932</v>
       </c>
       <c r="C40" s="414">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D40" s="412" t="s">
-        <v>34</v>
+        <v>730</v>
       </c>
       <c r="E40" s="412" t="s">
-        <v>938</v>
+        <v>933</v>
       </c>
       <c r="F40" s="412" t="s">
-        <v>1387</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="413" t="s">
-        <v>1012</v>
+        <v>1213</v>
       </c>
       <c r="B41" s="412" t="s">
-        <v>932</v>
+        <v>934</v>
       </c>
       <c r="C41" s="414">
-        <v>1</v>
-      </c>
-      <c r="D41" s="412" t="s">
-        <v>730</v>
+        <v>3</v>
       </c>
       <c r="E41" s="412" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="F41" s="412" t="s">
-        <v>1370</v>
+        <v>417</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="413" t="s">
-        <v>1013</v>
+        <v>1214</v>
       </c>
       <c r="B42" s="412" t="s">
         <v>934</v>
@@ -28716,19 +28782,16 @@
       <c r="C42" s="414">
         <v>3</v>
       </c>
-      <c r="D42" s="412" t="s">
-        <v>64</v>
-      </c>
       <c r="E42" s="412" t="s">
-        <v>931</v>
+        <v>964</v>
       </c>
       <c r="F42" s="412" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="413" t="s">
-        <v>1419</v>
+        <v>1014</v>
       </c>
       <c r="B43" s="412" t="s">
         <v>935</v>
@@ -28745,24 +28808,27 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="413" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B44" s="412" t="s">
+        <v>1155</v>
+      </c>
+      <c r="C44" s="414">
+        <v>3</v>
+      </c>
+      <c r="D44" s="412" t="s">
         <v>1421</v>
       </c>
-      <c r="B44" s="412" t="s">
-        <v>935</v>
-      </c>
-      <c r="C44" s="414">
-        <v>1</v>
-      </c>
       <c r="E44" s="412" t="s">
-        <v>1034</v>
+        <v>942</v>
       </c>
       <c r="F44" s="412" t="s">
-        <v>189</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="413" t="s">
-        <v>1154</v>
+        <v>1156</v>
       </c>
       <c r="B45" s="412" t="s">
         <v>1155</v>
@@ -28770,62 +28836,62 @@
       <c r="C45" s="414">
         <v>3</v>
       </c>
+      <c r="D45" s="412" t="s">
+        <v>1421</v>
+      </c>
       <c r="E45" s="412" t="s">
-        <v>942</v>
+        <v>938</v>
       </c>
       <c r="F45" s="412" t="s">
-        <v>432</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="413" t="s">
-        <v>1156</v>
+        <v>1015</v>
       </c>
       <c r="B46" s="412" t="s">
-        <v>1155</v>
+        <v>1334</v>
       </c>
       <c r="C46" s="414">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E46" s="412" t="s">
-        <v>938</v>
+        <v>1329</v>
       </c>
       <c r="F46" s="412" t="s">
-        <v>432</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="413" t="s">
-        <v>1172</v>
+        <v>1016</v>
       </c>
       <c r="B47" s="412" t="s">
-        <v>1155</v>
+        <v>1334</v>
       </c>
       <c r="C47" s="414">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E47" s="412" t="s">
-        <v>1193</v>
+        <v>1210</v>
       </c>
       <c r="F47" s="412" t="s">
-        <v>432</v>
+        <v>100</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="413" t="s">
-        <v>1015</v>
+        <v>1196</v>
       </c>
       <c r="B48" s="412" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="C48" s="414">
         <v>2</v>
       </c>
-      <c r="D48" s="412" t="s">
-        <v>743</v>
-      </c>
       <c r="E48" s="412" t="s">
-        <v>1423</v>
+        <v>1497</v>
       </c>
       <c r="F48" s="412" t="s">
         <v>100</v>
@@ -28833,19 +28899,16 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="413" t="s">
-        <v>1016</v>
+        <v>1198</v>
       </c>
       <c r="B49" s="412" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="C49" s="414">
         <v>1</v>
       </c>
-      <c r="D49" s="412" t="s">
-        <v>743</v>
-      </c>
       <c r="E49" s="412" t="s">
-        <v>919</v>
+        <v>1034</v>
       </c>
       <c r="F49" s="412" t="s">
         <v>100</v>
@@ -28853,87 +28916,78 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="413" t="s">
-        <v>1196</v>
+        <v>1017</v>
       </c>
       <c r="B50" s="412" t="s">
-        <v>1335</v>
+        <v>939</v>
       </c>
       <c r="C50" s="414">
-        <v>2</v>
-      </c>
-      <c r="D50" s="412" t="s">
-        <v>741</v>
+        <v>1</v>
       </c>
       <c r="E50" s="412" t="s">
-        <v>1203</v>
+        <v>919</v>
       </c>
       <c r="F50" s="412" t="s">
-        <v>100</v>
+        <v>24</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="413" t="s">
-        <v>1198</v>
+        <v>1018</v>
       </c>
       <c r="B51" s="412" t="s">
-        <v>1335</v>
+        <v>980</v>
       </c>
       <c r="C51" s="414">
-        <v>1</v>
-      </c>
-      <c r="D51" s="412" t="s">
-        <v>741</v>
+        <v>3</v>
       </c>
       <c r="E51" s="412" t="s">
-        <v>1034</v>
+        <v>942</v>
       </c>
       <c r="F51" s="412" t="s">
-        <v>100</v>
+        <v>417</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="413" t="s">
-        <v>1017</v>
+        <v>1019</v>
       </c>
       <c r="B52" s="412" t="s">
-        <v>939</v>
+        <v>943</v>
       </c>
       <c r="C52" s="414">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D52" s="412" t="s">
-        <v>741</v>
+        <v>184</v>
       </c>
       <c r="E52" s="412" t="s">
-        <v>916</v>
+        <v>1498</v>
       </c>
       <c r="F52" s="412" t="s">
-        <v>24</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="413" t="s">
-        <v>1018</v>
+        <v>1020</v>
       </c>
       <c r="B53" s="412" t="s">
-        <v>980</v>
+        <v>943</v>
       </c>
       <c r="C53" s="414">
-        <v>3</v>
-      </c>
-      <c r="D53" s="412" t="s">
-        <v>64</v>
+        <v>1</v>
       </c>
       <c r="E53" s="412" t="s">
-        <v>942</v>
+        <v>1490</v>
       </c>
       <c r="F53" s="412" t="s">
-        <v>129</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="413" t="s">
-        <v>1019</v>
+        <v>1161</v>
       </c>
       <c r="B54" s="412" t="s">
         <v>943</v>
@@ -28945,15 +28999,15 @@
         <v>184</v>
       </c>
       <c r="E54" s="412" t="s">
-        <v>944</v>
+        <v>1498</v>
       </c>
       <c r="F54" s="412" t="s">
-        <v>1424</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="413" t="s">
-        <v>1020</v>
+        <v>1163</v>
       </c>
       <c r="B55" s="412" t="s">
         <v>943</v>
@@ -28961,122 +29015,113 @@
       <c r="C55" s="414">
         <v>1</v>
       </c>
-      <c r="D55" s="412" t="s">
-        <v>1219</v>
-      </c>
       <c r="E55" s="412" t="s">
-        <v>1337</v>
+        <v>1486</v>
       </c>
       <c r="F55" s="412" t="s">
-        <v>104</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="413" t="s">
-        <v>1161</v>
+        <v>1074</v>
       </c>
       <c r="B56" s="412" t="s">
-        <v>943</v>
+        <v>945</v>
       </c>
       <c r="C56" s="414">
-        <v>2</v>
-      </c>
-      <c r="D56" s="412" t="s">
-        <v>184</v>
+        <v>3</v>
       </c>
       <c r="E56" s="412" t="s">
-        <v>1062</v>
+        <v>946</v>
       </c>
       <c r="F56" s="412" t="s">
-        <v>129</v>
+        <v>417</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="413" t="s">
-        <v>1163</v>
+        <v>1022</v>
       </c>
       <c r="B57" s="412" t="s">
-        <v>943</v>
+        <v>981</v>
       </c>
       <c r="C57" s="414">
-        <v>1</v>
-      </c>
-      <c r="D57" s="412" t="s">
-        <v>1219</v>
+        <v>3</v>
       </c>
       <c r="E57" s="412" t="s">
-        <v>1337</v>
+        <v>947</v>
       </c>
       <c r="F57" s="412" t="s">
-        <v>24</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="413" t="s">
-        <v>1074</v>
+        <v>1023</v>
       </c>
       <c r="B58" s="412" t="s">
-        <v>945</v>
+        <v>951</v>
       </c>
       <c r="C58" s="414">
         <v>3</v>
       </c>
       <c r="D58" s="412" t="s">
-        <v>732</v>
+        <v>872</v>
       </c>
       <c r="E58" s="412" t="s">
-        <v>946</v>
+        <v>950</v>
       </c>
       <c r="F58" s="412" t="s">
-        <v>293</v>
+        <v>189</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="413" t="s">
-        <v>1022</v>
+        <v>1024</v>
       </c>
       <c r="B59" s="412" t="s">
-        <v>981</v>
+        <v>952</v>
       </c>
       <c r="C59" s="414">
         <v>3</v>
       </c>
       <c r="D59" s="412" t="s">
-        <v>414</v>
+        <v>872</v>
       </c>
       <c r="E59" s="412" t="s">
-        <v>947</v>
+        <v>972</v>
       </c>
       <c r="F59" s="412" t="s">
-        <v>50</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="413" t="s">
-        <v>1338</v>
+        <v>1025</v>
       </c>
       <c r="B60" s="412" t="s">
-        <v>1339</v>
+        <v>954</v>
       </c>
       <c r="C60" s="414">
         <v>3</v>
       </c>
       <c r="D60" s="412" t="s">
-        <v>138</v>
+        <v>658</v>
       </c>
       <c r="E60" s="412" t="s">
-        <v>946</v>
+        <v>914</v>
       </c>
       <c r="F60" s="412" t="s">
-        <v>215</v>
+        <v>189</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="413" t="s">
-        <v>1023</v>
+        <v>1026</v>
       </c>
       <c r="B61" s="412" t="s">
-        <v>951</v>
+        <v>982</v>
       </c>
       <c r="C61" s="414">
         <v>3</v>
@@ -29085,7 +29130,7 @@
         <v>872</v>
       </c>
       <c r="E61" s="412" t="s">
-        <v>950</v>
+        <v>947</v>
       </c>
       <c r="F61" s="412" t="s">
         <v>189</v>
@@ -29093,416 +29138,295 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="413" t="s">
-        <v>1024</v>
+        <v>1078</v>
       </c>
       <c r="B62" s="412" t="s">
-        <v>952</v>
+        <v>956</v>
       </c>
       <c r="C62" s="414">
         <v>3</v>
       </c>
-      <c r="D62" s="412" t="s">
-        <v>607</v>
-      </c>
       <c r="E62" s="412" t="s">
-        <v>962</v>
+        <v>946</v>
       </c>
       <c r="F62" s="412" t="s">
-        <v>129</v>
+        <v>100</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="413" t="s">
-        <v>1025</v>
+        <v>1079</v>
       </c>
       <c r="B63" s="412" t="s">
-        <v>954</v>
+        <v>957</v>
       </c>
       <c r="C63" s="414">
         <v>3</v>
       </c>
       <c r="D63" s="412" t="s">
-        <v>658</v>
+        <v>481</v>
       </c>
       <c r="E63" s="412" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F63" s="412" t="s">
-        <v>189</v>
+        <v>100</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="413" t="s">
-        <v>1026</v>
+        <v>1339</v>
       </c>
       <c r="B64" s="412" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="C64" s="414">
         <v>3</v>
       </c>
       <c r="D64" s="412" t="s">
-        <v>872</v>
+        <v>743</v>
       </c>
       <c r="E64" s="412" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="F64" s="412" t="s">
-        <v>189</v>
+        <v>77</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="413" t="s">
-        <v>1078</v>
+        <v>1032</v>
       </c>
       <c r="B65" s="412" t="s">
-        <v>956</v>
+        <v>1180</v>
       </c>
       <c r="C65" s="414">
         <v>3</v>
       </c>
-      <c r="D65" s="412" t="s">
-        <v>811</v>
-      </c>
       <c r="E65" s="412" t="s">
-        <v>946</v>
+        <v>962</v>
       </c>
       <c r="F65" s="412" t="s">
-        <v>129</v>
+        <v>432</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="413" t="s">
-        <v>1079</v>
+        <v>1033</v>
       </c>
       <c r="B66" s="412" t="s">
-        <v>957</v>
+        <v>984</v>
       </c>
       <c r="C66" s="414">
         <v>3</v>
       </c>
       <c r="E66" s="412" t="s">
-        <v>928</v>
+        <v>972</v>
       </c>
       <c r="F66" s="412" t="s">
-        <v>119</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="413" t="s">
-        <v>1340</v>
+        <v>1083</v>
       </c>
       <c r="B67" s="412" t="s">
-        <v>983</v>
+        <v>1183</v>
       </c>
       <c r="C67" s="414">
-        <v>3</v>
-      </c>
-      <c r="D67" s="412" t="s">
-        <v>743</v>
+        <v>1</v>
       </c>
       <c r="E67" s="412" t="s">
-        <v>950</v>
+        <v>1207</v>
       </c>
       <c r="F67" s="412" t="s">
-        <v>215</v>
+        <v>135</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="413" t="s">
-        <v>1032</v>
+        <v>1340</v>
       </c>
       <c r="B68" s="412" t="s">
-        <v>1180</v>
+        <v>1341</v>
       </c>
       <c r="C68" s="414">
         <v>3</v>
       </c>
-      <c r="D68" s="412" t="s">
-        <v>64</v>
-      </c>
       <c r="E68" s="412" t="s">
-        <v>962</v>
+        <v>972</v>
       </c>
       <c r="F68" s="412" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="413" t="s">
-        <v>1033</v>
+        <v>1035</v>
       </c>
       <c r="B69" s="412" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C69" s="414">
         <v>3</v>
       </c>
       <c r="D69" s="412" t="s">
-        <v>166</v>
+        <v>184</v>
       </c>
       <c r="E69" s="412" t="s">
-        <v>972</v>
+        <v>942</v>
       </c>
       <c r="F69" s="412" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="413" t="s">
-        <v>1083</v>
+        <v>1342</v>
       </c>
       <c r="B70" s="412" t="s">
-        <v>1183</v>
+        <v>986</v>
       </c>
       <c r="C70" s="414">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D70" s="412" t="s">
-        <v>888</v>
+        <v>604</v>
       </c>
       <c r="E70" s="412" t="s">
-        <v>1207</v>
+        <v>1504</v>
       </c>
       <c r="F70" s="412" t="s">
-        <v>135</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="413" t="s">
-        <v>1341</v>
+        <v>1220</v>
       </c>
       <c r="B71" s="412" t="s">
-        <v>1342</v>
+        <v>1186</v>
       </c>
       <c r="C71" s="414">
         <v>3</v>
       </c>
-      <c r="D71" s="412" t="s">
-        <v>64</v>
-      </c>
       <c r="E71" s="412" t="s">
-        <v>972</v>
+        <v>958</v>
       </c>
       <c r="F71" s="412" t="s">
-        <v>24</v>
+        <v>189</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="413" t="s">
-        <v>1035</v>
+        <v>1040</v>
       </c>
       <c r="B72" s="412" t="s">
-        <v>985</v>
+        <v>989</v>
       </c>
       <c r="C72" s="414">
         <v>3</v>
       </c>
-      <c r="D72" s="412" t="s">
-        <v>184</v>
-      </c>
       <c r="E72" s="412" t="s">
-        <v>942</v>
+        <v>972</v>
       </c>
       <c r="F72" s="412" t="s">
-        <v>119</v>
+        <v>77</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="413" t="s">
-        <v>1343</v>
+        <v>1367</v>
       </c>
       <c r="B73" s="412" t="s">
-        <v>986</v>
+        <v>990</v>
       </c>
       <c r="C73" s="414">
         <v>3</v>
       </c>
-      <c r="D73" s="412" t="s">
-        <v>604</v>
-      </c>
       <c r="E73" s="412" t="s">
-        <v>1396</v>
+        <v>964</v>
       </c>
       <c r="F73" s="412" t="s">
-        <v>1225</v>
+        <v>77</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="413" t="s">
-        <v>1348</v>
+        <v>1043</v>
       </c>
       <c r="B74" s="412" t="s">
-        <v>988</v>
+        <v>992</v>
       </c>
       <c r="C74" s="414">
         <v>3</v>
       </c>
+      <c r="D74" s="412" t="s">
+        <v>658</v>
+      </c>
       <c r="E74" s="412" t="s">
-        <v>964</v>
+        <v>946</v>
       </c>
       <c r="F74" s="412" t="s">
-        <v>215</v>
+        <v>189</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="413" t="s">
-        <v>1220</v>
+        <v>1096</v>
       </c>
       <c r="B75" s="412" t="s">
-        <v>1186</v>
+        <v>1097</v>
       </c>
       <c r="C75" s="414">
         <v>3</v>
       </c>
       <c r="D75" s="412" t="s">
-        <v>166</v>
+        <v>872</v>
       </c>
       <c r="E75" s="412" t="s">
-        <v>958</v>
+        <v>924</v>
       </c>
       <c r="F75" s="412" t="s">
-        <v>293</v>
+        <v>189</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="413" t="s">
-        <v>1040</v>
+        <v>1343</v>
       </c>
       <c r="B76" s="412" t="s">
-        <v>989</v>
+        <v>1181</v>
       </c>
       <c r="C76" s="414">
         <v>3</v>
       </c>
       <c r="D76" s="412" t="s">
-        <v>414</v>
+        <v>59</v>
       </c>
       <c r="E76" s="412" t="s">
-        <v>972</v>
+        <v>947</v>
       </c>
       <c r="F76" s="412" t="s">
-        <v>77</v>
+        <v>123</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="413" t="s">
-        <v>1041</v>
+        <v>1046</v>
       </c>
       <c r="B77" s="412" t="s">
-        <v>990</v>
+        <v>993</v>
       </c>
       <c r="C77" s="414">
         <v>3</v>
       </c>
-      <c r="D77" s="412" t="s">
-        <v>45</v>
-      </c>
       <c r="E77" s="412" t="s">
-        <v>964</v>
+        <v>969</v>
       </c>
       <c r="F77" s="412" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78" s="413" t="s">
-        <v>1042</v>
-      </c>
-      <c r="B78" s="412" t="s">
-        <v>991</v>
-      </c>
-      <c r="C78" s="414">
-        <v>3</v>
-      </c>
-      <c r="D78" s="412" t="s">
-        <v>1218</v>
-      </c>
-      <c r="E78" s="412" t="s">
-        <v>928</v>
-      </c>
-      <c r="F78" s="412" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79" s="413" t="s">
-        <v>1043</v>
-      </c>
-      <c r="B79" s="412" t="s">
-        <v>992</v>
-      </c>
-      <c r="C79" s="414">
-        <v>3</v>
-      </c>
-      <c r="D79" s="412" t="s">
-        <v>658</v>
-      </c>
-      <c r="E79" s="412" t="s">
-        <v>946</v>
-      </c>
-      <c r="F79" s="412" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80" s="413" t="s">
-        <v>1096</v>
-      </c>
-      <c r="B80" s="412" t="s">
-        <v>1097</v>
-      </c>
-      <c r="C80" s="414">
-        <v>3</v>
-      </c>
-      <c r="D80" s="412" t="s">
-        <v>872</v>
-      </c>
-      <c r="E80" s="412" t="s">
-        <v>972</v>
-      </c>
-      <c r="F80" s="412" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A81" s="413" t="s">
-        <v>1344</v>
-      </c>
-      <c r="B81" s="412" t="s">
-        <v>1181</v>
-      </c>
-      <c r="C81" s="414">
-        <v>3</v>
-      </c>
-      <c r="D81" s="412" t="s">
-        <v>59</v>
-      </c>
-      <c r="E81" s="412" t="s">
-        <v>947</v>
-      </c>
-      <c r="F81" s="412" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A82" s="413" t="s">
-        <v>1046</v>
-      </c>
-      <c r="B82" s="412" t="s">
-        <v>993</v>
-      </c>
-      <c r="C82" s="414">
-        <v>3</v>
-      </c>
-      <c r="D82" s="412" t="s">
-        <v>1219</v>
-      </c>
-      <c r="E82" s="412" t="s">
-        <v>969</v>
-      </c>
-      <c r="F82" s="412" t="s">
-        <v>215</v>
+        <v>432</v>
       </c>
     </row>
   </sheetData>
@@ -37631,13 +37555,13 @@
   <sheetPr codeName="Sheet44">
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" ySplit="12" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="B42" sqref="B42"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -37653,7 +37577,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="410" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="407" t="s">
-        <v>1113</v>
+        <v>1483</v>
       </c>
       <c r="B1" s="408"/>
       <c r="C1" s="409"/>
@@ -37662,17 +37586,17 @@
       </c>
       <c r="E1" s="418"/>
       <c r="F1" s="458" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="410" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="409"/>
       <c r="C2" s="409"/>
       <c r="D2" s="449" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="E2" s="449" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="F2" s="458"/>
     </row>
@@ -37683,7 +37607,7 @@
         <v>1110</v>
       </c>
       <c r="E3" s="449" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="F3" s="449"/>
     </row>
@@ -37694,10 +37618,10 @@
       <c r="B4" s="457"/>
       <c r="C4" s="457"/>
       <c r="D4" s="449" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="E4" s="449" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="F4" s="449"/>
     </row>
@@ -37717,24 +37641,29 @@
     </row>
     <row r="7" spans="1:6" s="410" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="457" t="s">
-        <v>1277</v>
+        <v>1479</v>
       </c>
       <c r="B7" s="457"/>
       <c r="C7" s="457"/>
-      <c r="D7" s="404"/>
-      <c r="E7" s="449"/>
-      <c r="F7" s="449"/>
+      <c r="D7" s="457"/>
+      <c r="E7" s="457"/>
+      <c r="F7" s="457"/>
     </row>
     <row r="8" spans="1:6" s="410" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="457"/>
       <c r="B8" s="457"/>
       <c r="C8" s="457"/>
-      <c r="D8" s="404"/>
-    </row>
-    <row r="9" spans="1:6" s="410" customFormat="1" ht="9" x14ac:dyDescent="0.15">
+      <c r="D8" s="457"/>
+      <c r="E8" s="457"/>
+      <c r="F8" s="457"/>
+    </row>
+    <row r="9" spans="1:6" s="410" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="457"/>
       <c r="B9" s="457"/>
       <c r="C9" s="457"/>
+      <c r="D9" s="457"/>
+      <c r="E9" s="457"/>
+      <c r="F9" s="457"/>
     </row>
     <row r="10" spans="1:6" s="410" customFormat="1" ht="9" x14ac:dyDescent="0.15">
       <c r="A10" s="409"/>
@@ -37772,7 +37701,7 @@
         <v>1001</v>
       </c>
       <c r="B13" s="412" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="C13" s="414">
         <v>3</v>
@@ -37789,79 +37718,79 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="413" t="s">
-        <v>1056</v>
+        <v>1397</v>
       </c>
       <c r="B14" s="412" t="s">
-        <v>915</v>
+        <v>982</v>
       </c>
       <c r="C14" s="414">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D14" s="412" t="s">
         <v>872</v>
       </c>
       <c r="E14" s="412" t="s">
-        <v>1380</v>
+        <v>1398</v>
       </c>
       <c r="F14" s="412" t="s">
-        <v>14</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="413" t="s">
-        <v>1057</v>
+        <v>1472</v>
       </c>
       <c r="B15" s="412" t="s">
-        <v>915</v>
+        <v>952</v>
       </c>
       <c r="C15" s="414">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D15" s="412" t="s">
-        <v>1417</v>
+        <v>872</v>
       </c>
       <c r="E15" s="412" t="s">
-        <v>933</v>
+        <v>1473</v>
       </c>
       <c r="F15" s="412" t="s">
-        <v>14</v>
+        <v>189</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="413" t="s">
-        <v>1058</v>
+        <v>1399</v>
       </c>
       <c r="B16" s="412" t="s">
-        <v>915</v>
+        <v>1407</v>
       </c>
       <c r="C16" s="414">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D16" s="412" t="s">
-        <v>1417</v>
+        <v>64</v>
       </c>
       <c r="E16" s="412" t="s">
-        <v>1210</v>
+        <v>1348</v>
       </c>
       <c r="F16" s="412" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="413" t="s">
-        <v>1002</v>
+        <v>1349</v>
       </c>
       <c r="B17" s="412" t="s">
-        <v>917</v>
+        <v>1474</v>
       </c>
       <c r="C17" s="414">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D17" s="412" t="s">
         <v>481</v>
       </c>
       <c r="E17" s="412" t="s">
-        <v>1426</v>
+        <v>1475</v>
       </c>
       <c r="F17" s="412" t="s">
         <v>100</v>
@@ -37869,269 +37798,59 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="413" t="s">
-        <v>1003</v>
+        <v>1476</v>
       </c>
       <c r="B18" s="412" t="s">
-        <v>917</v>
+        <v>1477</v>
       </c>
       <c r="C18" s="414">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D18" s="412" t="s">
-        <v>481</v>
+        <v>658</v>
       </c>
       <c r="E18" s="412" t="s">
-        <v>916</v>
+        <v>1478</v>
       </c>
       <c r="F18" s="412" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="413" t="s">
-        <v>1059</v>
-      </c>
-      <c r="B19" s="412" t="s">
-        <v>917</v>
-      </c>
-      <c r="C19" s="414">
-        <v>2</v>
-      </c>
-      <c r="D19" s="412" t="s">
-        <v>481</v>
-      </c>
-      <c r="E19" s="412" t="s">
-        <v>1427</v>
-      </c>
-      <c r="F19" s="412" t="s">
-        <v>100</v>
+        <v>189</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="413" t="s">
-        <v>1060</v>
-      </c>
       <c r="B20" s="412" t="s">
-        <v>917</v>
-      </c>
-      <c r="C20" s="414">
-        <v>1</v>
-      </c>
-      <c r="D20" s="412" t="s">
-        <v>481</v>
-      </c>
-      <c r="E20" s="412" t="s">
-        <v>1331</v>
-      </c>
-      <c r="F20" s="412" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="413" t="s">
-        <v>1061</v>
-      </c>
-      <c r="B21" s="412" t="s">
-        <v>917</v>
-      </c>
-      <c r="C21" s="414">
-        <v>2</v>
-      </c>
-      <c r="D21" s="412" t="s">
-        <v>59</v>
-      </c>
-      <c r="E21" s="412" t="s">
-        <v>1428</v>
-      </c>
-      <c r="F21" s="412" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="413" t="s">
-        <v>1063</v>
-      </c>
-      <c r="B22" s="412" t="s">
-        <v>917</v>
-      </c>
-      <c r="C22" s="414">
-        <v>1</v>
-      </c>
-      <c r="D22" s="412" t="s">
-        <v>59</v>
-      </c>
-      <c r="E22" s="412" t="s">
-        <v>1333</v>
-      </c>
-      <c r="F22" s="412" t="s">
-        <v>100</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="413" t="s">
-        <v>1064</v>
-      </c>
       <c r="B23" s="412" t="s">
-        <v>920</v>
-      </c>
-      <c r="C23" s="414">
-        <v>1</v>
-      </c>
-      <c r="D23" s="412" t="s">
-        <v>743</v>
-      </c>
-      <c r="E23" s="412" t="s">
-        <v>919</v>
-      </c>
-      <c r="F23" s="412" t="s">
-        <v>19</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="413" t="s">
-        <v>1065</v>
+        <v>1482</v>
       </c>
       <c r="B24" s="412" t="s">
-        <v>920</v>
+        <v>1191</v>
       </c>
       <c r="C24" s="414">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D24" s="412" t="s">
-        <v>1366</v>
+        <v>912</v>
       </c>
       <c r="E24" s="412" t="s">
-        <v>936</v>
+        <v>1402</v>
       </c>
       <c r="F24" s="412" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="413" t="s">
-        <v>1066</v>
-      </c>
-      <c r="B25" s="412" t="s">
-        <v>920</v>
-      </c>
-      <c r="C25" s="414">
-        <v>1</v>
-      </c>
-      <c r="D25" s="412" t="s">
-        <v>1366</v>
-      </c>
-      <c r="E25" s="412" t="s">
-        <v>1034</v>
-      </c>
-      <c r="F25" s="412" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="413" t="s">
-        <v>1381</v>
-      </c>
-      <c r="B26" s="412" t="s">
-        <v>920</v>
-      </c>
-      <c r="C26" s="414">
-        <v>1</v>
-      </c>
-      <c r="D26" s="412" t="s">
-        <v>811</v>
-      </c>
-      <c r="E26" s="412" t="s">
-        <v>1382</v>
-      </c>
-      <c r="F26" s="412" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="413" t="s">
-        <v>1383</v>
-      </c>
-      <c r="B27" s="412" t="s">
-        <v>920</v>
-      </c>
-      <c r="C27" s="414">
-        <v>1</v>
-      </c>
-      <c r="D27" s="412" t="s">
-        <v>811</v>
-      </c>
-      <c r="E27" s="412" t="s">
-        <v>1384</v>
-      </c>
-      <c r="F27" s="412" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="413" t="s">
-        <v>1004</v>
-      </c>
-      <c r="B28" s="412" t="s">
-        <v>921</v>
-      </c>
-      <c r="C28" s="414">
-        <v>2</v>
-      </c>
-      <c r="D28" s="412" t="s">
-        <v>159</v>
-      </c>
-      <c r="E28" s="412" t="s">
-        <v>1379</v>
-      </c>
-      <c r="F28" s="412" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="413" t="s">
-        <v>1005</v>
-      </c>
-      <c r="B29" s="412" t="s">
-        <v>921</v>
-      </c>
-      <c r="C29" s="414">
-        <v>1</v>
-      </c>
-      <c r="D29" s="412" t="s">
-        <v>159</v>
-      </c>
-      <c r="E29" s="412" t="s">
-        <v>1171</v>
-      </c>
-      <c r="F29" s="412" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="413" t="s">
-        <v>1168</v>
-      </c>
-      <c r="B30" s="412" t="s">
-        <v>921</v>
-      </c>
-      <c r="C30" s="414">
-        <v>2</v>
-      </c>
-      <c r="D30" s="412" t="s">
-        <v>743</v>
-      </c>
-      <c r="E30" s="412" t="s">
-        <v>1429</v>
-      </c>
-      <c r="F30" s="412" t="s">
-        <v>100</v>
+        <v>432</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A4:C6"/>
-    <mergeCell ref="A7:C9"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A7:F9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D1" r:id="rId1"/>
@@ -41860,7 +41579,7 @@
     <row r="1" spans="1:6" s="410" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="407"/>
       <c r="B1" s="456" t="s">
-        <v>1467</v>
+        <v>1465</v>
       </c>
       <c r="C1" s="409"/>
       <c r="D1" s="418" t="s">
@@ -41868,17 +41587,17 @@
       </c>
       <c r="E1" s="418"/>
       <c r="F1" s="458" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="410" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="409"/>
       <c r="C2" s="409"/>
       <c r="D2" s="449" t="s">
+        <v>1279</v>
+      </c>
+      <c r="E2" s="449" t="s">
         <v>1280</v>
-      </c>
-      <c r="E2" s="449" t="s">
-        <v>1281</v>
       </c>
       <c r="F2" s="458"/>
     </row>
@@ -41886,7 +41605,7 @@
       <c r="B3" s="409"/>
       <c r="C3" s="409"/>
       <c r="D3" s="449" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="E3" s="449" t="s">
         <v>1136</v>
@@ -41900,10 +41619,10 @@
       <c r="B4" s="461"/>
       <c r="C4" s="461"/>
       <c r="D4" s="449" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="E4" s="449" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="F4" s="449"/>
     </row>
@@ -41912,10 +41631,10 @@
       <c r="B5" s="461"/>
       <c r="C5" s="461"/>
       <c r="D5" s="449" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="E5" s="449" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="410" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
@@ -41923,7 +41642,7 @@
       <c r="B6" s="461"/>
       <c r="C6" s="461"/>
       <c r="D6" s="449" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="E6" s="449" t="s">
         <v>1230</v>
@@ -41932,15 +41651,15 @@
     </row>
     <row r="7" spans="1:6" s="410" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="461" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="B7" s="461"/>
       <c r="C7" s="461"/>
       <c r="D7" s="449" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="E7" s="449" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="F7" s="449"/>
     </row>
@@ -41949,7 +41668,7 @@
       <c r="B8" s="461"/>
       <c r="C8" s="461"/>
       <c r="D8" s="449" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="E8" s="449" t="s">
         <v>1102</v>
@@ -41960,10 +41679,10 @@
       <c r="B9" s="461"/>
       <c r="C9" s="461"/>
       <c r="D9" s="449" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="E9" s="449" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="410" customFormat="1" ht="9" x14ac:dyDescent="0.15">
@@ -42003,7 +41722,7 @@
         <v>1001</v>
       </c>
       <c r="B13" s="412" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="C13" s="414">
         <v>3</v>
@@ -42032,7 +41751,7 @@
         <v>872</v>
       </c>
       <c r="E14" s="412" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="F14" s="412" t="s">
         <v>14</v>
@@ -42049,7 +41768,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="412" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
       <c r="E15" s="412" t="s">
         <v>933</v>
@@ -42080,7 +41799,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="413" t="s">
-        <v>1459</v>
+        <v>1457</v>
       </c>
       <c r="B17" s="412" t="s">
         <v>915</v>
@@ -42112,7 +41831,7 @@
         <v>481</v>
       </c>
       <c r="E18" s="412" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="F18" s="412" t="s">
         <v>100</v>
@@ -42132,7 +41851,7 @@
         <v>481</v>
       </c>
       <c r="E19" s="412" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="F19" s="412" t="s">
         <v>100</v>
@@ -42152,7 +41871,7 @@
         <v>59</v>
       </c>
       <c r="E20" s="412" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="F20" s="412" t="s">
         <v>100</v>
@@ -42172,7 +41891,7 @@
         <v>59</v>
       </c>
       <c r="E21" s="412" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="F21" s="412" t="s">
         <v>100</v>
@@ -42209,7 +41928,7 @@
         <v>1</v>
       </c>
       <c r="D23" s="412" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="E23" s="412" t="s">
         <v>936</v>
@@ -42220,7 +41939,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="413" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="B24" s="412" t="s">
         <v>920</v>
@@ -42232,7 +41951,7 @@
         <v>811</v>
       </c>
       <c r="E24" s="412" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="F24" s="412" t="s">
         <v>19</v>
@@ -42240,7 +41959,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="413" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="B25" s="412" t="s">
         <v>920</v>
@@ -42252,7 +41971,7 @@
         <v>811</v>
       </c>
       <c r="E25" s="412" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="F25" s="412" t="s">
         <v>19</v>
@@ -42272,7 +41991,7 @@
         <v>159</v>
       </c>
       <c r="E26" s="412" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="F26" s="412" t="s">
         <v>100</v>
@@ -42312,7 +42031,7 @@
         <v>481</v>
       </c>
       <c r="E28" s="412" t="s">
-        <v>1430</v>
+        <v>1428</v>
       </c>
       <c r="F28" s="412" t="s">
         <v>100</v>
@@ -42332,7 +42051,7 @@
         <v>481</v>
       </c>
       <c r="E29" s="412" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="F29" s="412" t="s">
         <v>100</v>
@@ -42372,7 +42091,7 @@
         <v>811</v>
       </c>
       <c r="E31" s="412" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="F31" s="412" t="s">
         <v>77</v>
@@ -42389,13 +42108,13 @@
         <v>3</v>
       </c>
       <c r="D32" s="412" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="E32" s="412" t="s">
         <v>958</v>
       </c>
       <c r="F32" s="412" t="s">
-        <v>1431</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -42415,15 +42134,15 @@
         <v>929</v>
       </c>
       <c r="F33" s="412" t="s">
-        <v>1431</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="413" t="s">
+        <v>1370</v>
+      </c>
+      <c r="B34" s="412" t="s">
         <v>1371</v>
-      </c>
-      <c r="B34" s="412" t="s">
-        <v>1372</v>
       </c>
       <c r="C34" s="414">
         <v>3</v>
@@ -42435,7 +42154,7 @@
         <v>914</v>
       </c>
       <c r="F34" s="412" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -42455,7 +42174,7 @@
         <v>931</v>
       </c>
       <c r="F35" s="412" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -42500,7 +42219,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="413" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="B38" s="412" t="s">
         <v>935</v>
@@ -42509,7 +42228,7 @@
         <v>1</v>
       </c>
       <c r="D38" s="412" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="E38" s="412" t="s">
         <v>936</v>
@@ -42520,7 +42239,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="413" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="B39" s="412" t="s">
         <v>935</v>
@@ -42549,13 +42268,13 @@
         <v>3</v>
       </c>
       <c r="D40" s="412" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="E40" s="412" t="s">
         <v>942</v>
       </c>
       <c r="F40" s="412" t="s">
-        <v>1460</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -42569,13 +42288,13 @@
         <v>3</v>
       </c>
       <c r="D41" s="412" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="E41" s="412" t="s">
         <v>938</v>
       </c>
       <c r="F41" s="412" t="s">
-        <v>1460</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -42589,13 +42308,13 @@
         <v>3</v>
       </c>
       <c r="D42" s="412" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="E42" s="412" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="F42" s="412" t="s">
-        <v>1460</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -42612,7 +42331,7 @@
         <v>741</v>
       </c>
       <c r="E43" s="412" t="s">
-        <v>1432</v>
+        <v>1430</v>
       </c>
       <c r="F43" s="412" t="s">
         <v>100</v>
@@ -42632,7 +42351,7 @@
         <v>741</v>
       </c>
       <c r="E44" s="412" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
       <c r="F44" s="412" t="s">
         <v>100</v>
@@ -42652,7 +42371,7 @@
         <v>741</v>
       </c>
       <c r="E45" s="412" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="F45" s="412" t="s">
         <v>100</v>
@@ -42692,7 +42411,7 @@
         <v>741</v>
       </c>
       <c r="E47" s="412" t="s">
-        <v>1434</v>
+        <v>1432</v>
       </c>
       <c r="F47" s="412" t="s">
         <v>100</v>
@@ -42735,7 +42454,7 @@
         <v>929</v>
       </c>
       <c r="F49" s="412" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -42755,7 +42474,7 @@
         <v>938</v>
       </c>
       <c r="F50" s="412" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -42789,7 +42508,7 @@
         <v>2</v>
       </c>
       <c r="D52" s="412" t="s">
-        <v>1466</v>
+        <v>1464</v>
       </c>
       <c r="E52" s="412" t="s">
         <v>944</v>
@@ -42809,13 +42528,13 @@
         <v>1</v>
       </c>
       <c r="D53" s="412" t="s">
-        <v>1442</v>
+        <v>1440</v>
       </c>
       <c r="E53" s="412" t="s">
         <v>916</v>
       </c>
       <c r="F53" s="412" t="s">
-        <v>1461</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -42829,7 +42548,7 @@
         <v>2</v>
       </c>
       <c r="D54" s="412" t="s">
-        <v>1466</v>
+        <v>1464</v>
       </c>
       <c r="E54" s="412" t="s">
         <v>944</v>
@@ -42840,7 +42559,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="413" t="s">
-        <v>1435</v>
+        <v>1433</v>
       </c>
       <c r="B55" s="412" t="s">
         <v>943</v>
@@ -42849,13 +42568,13 @@
         <v>1</v>
       </c>
       <c r="D55" s="412" t="s">
-        <v>1442</v>
+        <v>1440</v>
       </c>
       <c r="E55" s="412" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="F55" s="412" t="s">
-        <v>1462</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
@@ -42900,16 +42619,16 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="413" t="s">
+        <v>1372</v>
+      </c>
+      <c r="B58" s="412" t="s">
         <v>1373</v>
-      </c>
-      <c r="B58" s="412" t="s">
-        <v>1374</v>
       </c>
       <c r="C58" s="414">
         <v>1</v>
       </c>
       <c r="D58" s="412" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="E58" s="412" t="s">
         <v>1210</v>
@@ -42935,7 +42654,7 @@
         <v>950</v>
       </c>
       <c r="F59" s="412" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -43060,10 +42779,10 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="413" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="B66" s="412" t="s">
-        <v>1436</v>
+        <v>1434</v>
       </c>
       <c r="C66" s="414">
         <v>3</v>
@@ -43083,7 +42802,7 @@
         <v>1082</v>
       </c>
       <c r="B67" s="412" t="s">
-        <v>1437</v>
+        <v>1435</v>
       </c>
       <c r="C67" s="414">
         <v>3</v>
@@ -43109,7 +42828,7 @@
         <v>1</v>
       </c>
       <c r="D68" s="412" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="E68" s="412" t="s">
         <v>1207</v>
@@ -43120,10 +42839,10 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="413" t="s">
-        <v>1464</v>
+        <v>1462</v>
       </c>
       <c r="B69" s="412" t="s">
-        <v>1465</v>
+        <v>1463</v>
       </c>
       <c r="C69" s="414">
         <v>3</v>
@@ -43140,10 +42859,10 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="413" t="s">
+        <v>1374</v>
+      </c>
+      <c r="B70" s="412" t="s">
         <v>1375</v>
-      </c>
-      <c r="B70" s="412" t="s">
-        <v>1376</v>
       </c>
       <c r="C70" s="414">
         <v>3</v>
@@ -43172,7 +42891,7 @@
         <v>604</v>
       </c>
       <c r="E71" s="412" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="F71" s="412" t="s">
         <v>1225</v>
@@ -43240,10 +42959,10 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="413" t="s">
-        <v>1457</v>
+        <v>1455</v>
       </c>
       <c r="B75" s="412" t="s">
-        <v>1458</v>
+        <v>1456</v>
       </c>
       <c r="C75" s="414">
         <v>3</v>
@@ -43360,7 +43079,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="410" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="407" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="B1" s="408"/>
       <c r="C1" s="409"/>
@@ -43369,17 +43088,17 @@
       </c>
       <c r="E1" s="418"/>
       <c r="F1" s="458" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="410" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="409"/>
       <c r="C2" s="409"/>
       <c r="D2" s="449" t="s">
+        <v>1299</v>
+      </c>
+      <c r="E2" s="449" t="s">
         <v>1300</v>
-      </c>
-      <c r="E2" s="449" t="s">
-        <v>1301</v>
       </c>
       <c r="F2" s="458"/>
     </row>
@@ -43387,7 +43106,7 @@
       <c r="B3" s="409"/>
       <c r="C3" s="409"/>
       <c r="D3" s="449" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="E3" s="449" t="s">
         <v>1227</v>
@@ -43401,7 +43120,7 @@
       <c r="B4" s="462"/>
       <c r="C4" s="462"/>
       <c r="D4" s="449" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="E4" s="449" t="s">
         <v>1228</v>
@@ -43413,7 +43132,7 @@
       <c r="B5" s="462"/>
       <c r="C5" s="462"/>
       <c r="D5" s="449" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="E5" s="449" t="s">
         <v>1229</v>
@@ -43425,7 +43144,7 @@
       <c r="B6" s="462"/>
       <c r="C6" s="462"/>
       <c r="D6" s="449" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="E6" s="449" t="s">
         <v>1230</v>
@@ -43434,12 +43153,12 @@
     </row>
     <row r="7" spans="1:6" s="410" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="462" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="B7" s="462"/>
       <c r="C7" s="462"/>
       <c r="D7" s="449" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="E7" s="449" t="s">
         <v>1231</v>
@@ -43451,7 +43170,7 @@
       <c r="B8" s="462"/>
       <c r="C8" s="462"/>
       <c r="D8" s="449" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="E8" s="449" t="s">
         <v>1101</v>
@@ -43463,10 +43182,10 @@
       <c r="B9" s="462"/>
       <c r="C9" s="462"/>
       <c r="D9" s="449" t="s">
+        <v>1307</v>
+      </c>
+      <c r="E9" s="449" t="s">
         <v>1308</v>
-      </c>
-      <c r="E9" s="449" t="s">
-        <v>1309</v>
       </c>
       <c r="F9" s="451"/>
     </row>
@@ -43509,7 +43228,7 @@
         <v>1001</v>
       </c>
       <c r="B13" s="412" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="C13" s="414">
         <v>3</v>
@@ -43521,7 +43240,7 @@
         <v>931</v>
       </c>
       <c r="F13" s="412" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -43535,10 +43254,10 @@
         <v>1</v>
       </c>
       <c r="D14" s="412" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
       <c r="E14" s="412" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="F14" s="412" t="s">
         <v>14</v>
@@ -43575,7 +43294,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="412" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
       <c r="E16" s="412" t="s">
         <v>1034</v>
@@ -43598,7 +43317,7 @@
         <v>481</v>
       </c>
       <c r="E17" s="412" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="F17" s="412" t="s">
         <v>119</v>
@@ -43618,7 +43337,7 @@
         <v>481</v>
       </c>
       <c r="E18" s="412" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="F18" s="412" t="s">
         <v>119</v>
@@ -43638,7 +43357,7 @@
         <v>481</v>
       </c>
       <c r="E19" s="412" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="F19" s="412" t="s">
         <v>119</v>
@@ -43735,7 +43454,7 @@
         <v>1</v>
       </c>
       <c r="D24" s="412" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="E24" s="412" t="s">
         <v>936</v>
@@ -43755,7 +43474,7 @@
         <v>1</v>
       </c>
       <c r="D25" s="412" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="E25" s="412" t="s">
         <v>1034</v>
@@ -43778,7 +43497,7 @@
         <v>481</v>
       </c>
       <c r="E26" s="412" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="F26" s="412" t="s">
         <v>100</v>
@@ -43798,7 +43517,7 @@
         <v>481</v>
       </c>
       <c r="E27" s="412" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="F27" s="412" t="s">
         <v>100</v>
@@ -43818,7 +43537,7 @@
         <v>811</v>
       </c>
       <c r="E28" s="412" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="F28" s="412" t="s">
         <v>100</v>
@@ -43838,7 +43557,7 @@
         <v>811</v>
       </c>
       <c r="E29" s="412" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="F29" s="412" t="s">
         <v>100</v>
@@ -43846,7 +43565,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="413" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="B30" s="412" t="s">
         <v>921</v>
@@ -43858,7 +43577,7 @@
         <v>741</v>
       </c>
       <c r="E30" s="412" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="F30" s="412" t="s">
         <v>100</v>
@@ -43866,7 +43585,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="413" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="B31" s="412" t="s">
         <v>921</v>
@@ -43878,7 +43597,7 @@
         <v>741</v>
       </c>
       <c r="E31" s="412" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="F31" s="412" t="s">
         <v>100</v>
@@ -43886,22 +43605,22 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="413" t="s">
+        <v>1390</v>
+      </c>
+      <c r="B32" s="412" t="s">
         <v>1391</v>
-      </c>
-      <c r="B32" s="412" t="s">
-        <v>1392</v>
       </c>
       <c r="C32" s="414">
         <v>3</v>
       </c>
       <c r="D32" s="412" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="E32" s="412" t="s">
         <v>929</v>
       </c>
       <c r="F32" s="412" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -43955,13 +43674,13 @@
         <v>3</v>
       </c>
       <c r="D35" s="412" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="E35" s="412" t="s">
         <v>972</v>
       </c>
       <c r="F35" s="412" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -43981,7 +43700,7 @@
         <v>929</v>
       </c>
       <c r="F36" s="412" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -43989,7 +43708,7 @@
         <v>1010</v>
       </c>
       <c r="B37" s="412" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="C37" s="414">
         <v>3</v>
@@ -44001,7 +43720,7 @@
         <v>914</v>
       </c>
       <c r="F37" s="412" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -44021,7 +43740,7 @@
         <v>938</v>
       </c>
       <c r="F38" s="412" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -44041,7 +43760,7 @@
         <v>933</v>
       </c>
       <c r="F39" s="412" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -44086,7 +43805,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="413" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="B42" s="412" t="s">
         <v>935</v>
@@ -44095,7 +43814,7 @@
         <v>1</v>
       </c>
       <c r="D42" s="412" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="E42" s="412" t="s">
         <v>936</v>
@@ -44106,7 +43825,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="413" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="B43" s="412" t="s">
         <v>935</v>
@@ -44115,7 +43834,7 @@
         <v>1</v>
       </c>
       <c r="D43" s="412" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="E43" s="412" t="s">
         <v>1034</v>
@@ -44135,7 +43854,7 @@
         <v>3</v>
       </c>
       <c r="D44" s="412" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="E44" s="412" t="s">
         <v>942</v>
@@ -44155,7 +43874,7 @@
         <v>3</v>
       </c>
       <c r="D45" s="412" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="E45" s="412" t="s">
         <v>938</v>
@@ -44169,7 +43888,7 @@
         <v>1015</v>
       </c>
       <c r="B46" s="412" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="C46" s="414">
         <v>2</v>
@@ -44178,7 +43897,7 @@
         <v>743</v>
       </c>
       <c r="E46" s="412" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="F46" s="412" t="s">
         <v>100</v>
@@ -44189,7 +43908,7 @@
         <v>1016</v>
       </c>
       <c r="B47" s="412" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="C47" s="414">
         <v>1</v>
@@ -44209,7 +43928,7 @@
         <v>1196</v>
       </c>
       <c r="B48" s="412" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="C48" s="414">
         <v>2</v>
@@ -44229,7 +43948,7 @@
         <v>1198</v>
       </c>
       <c r="B49" s="412" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="C49" s="414">
         <v>1</v>
@@ -44301,7 +44020,7 @@
         <v>944</v>
       </c>
       <c r="F52" s="412" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -44318,7 +44037,7 @@
         <v>1219</v>
       </c>
       <c r="E53" s="412" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="F53" s="412" t="s">
         <v>104</v>
@@ -44358,7 +44077,7 @@
         <v>1219</v>
       </c>
       <c r="E55" s="412" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="F55" s="412" t="s">
         <v>24</v>
@@ -44526,7 +44245,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="413" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="B64" s="412" t="s">
         <v>983</v>
@@ -44606,10 +44325,10 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="413" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B68" s="412" t="s">
         <v>1341</v>
-      </c>
-      <c r="B68" s="412" t="s">
-        <v>1342</v>
       </c>
       <c r="C68" s="414">
         <v>3</v>
@@ -44646,7 +44365,7 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="413" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="B70" s="412" t="s">
         <v>986</v>
@@ -44658,7 +44377,7 @@
         <v>604</v>
       </c>
       <c r="E70" s="412" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="F70" s="412" t="s">
         <v>1225</v>
@@ -44786,7 +44505,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="413" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="B77" s="412" t="s">
         <v>1181</v>
@@ -44815,7 +44534,7 @@
         <v>3</v>
       </c>
       <c r="D78" s="412" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="E78" s="412" t="s">
         <v>969</v>
@@ -44874,17 +44593,17 @@
       </c>
       <c r="E1" s="418"/>
       <c r="F1" s="458" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="410" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="409"/>
       <c r="C2" s="409"/>
       <c r="D2" s="454" t="s">
+        <v>1294</v>
+      </c>
+      <c r="E2" s="454" t="s">
         <v>1295</v>
-      </c>
-      <c r="E2" s="454" t="s">
-        <v>1296</v>
       </c>
       <c r="F2" s="458"/>
     </row>
@@ -44895,7 +44614,7 @@
         <v>43284</v>
       </c>
       <c r="E3" s="454" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="F3" s="454"/>
     </row>
@@ -44909,7 +44628,7 @@
         <v>1110</v>
       </c>
       <c r="E4" s="454" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="F4" s="454"/>
     </row>
@@ -44918,10 +44637,10 @@
       <c r="B5" s="463"/>
       <c r="C5" s="463"/>
       <c r="D5" s="404" t="s">
+        <v>1297</v>
+      </c>
+      <c r="E5" s="410" t="s">
         <v>1298</v>
-      </c>
-      <c r="E5" s="410" t="s">
-        <v>1299</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="410" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
@@ -44934,7 +44653,7 @@
     </row>
     <row r="7" spans="1:6" s="410" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="463" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="B7" s="463"/>
       <c r="C7" s="463"/>
@@ -44986,12 +44705,12 @@
     </row>
     <row r="13" spans="1:6" ht="12" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B13" s="412" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="413" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="B14" s="412" t="s">
         <v>982</v>
@@ -45003,7 +44722,7 @@
         <v>872</v>
       </c>
       <c r="E14" s="412" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="F14" s="412" t="s">
         <v>189</v>
@@ -45011,15 +44730,15 @@
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="412" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="413" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="B17" s="412" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="C17" s="414">
         <v>3</v>
@@ -45028,20 +44747,20 @@
         <v>64</v>
       </c>
       <c r="E17" s="412" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="F17" s="412" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B19" s="412" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="413" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="B20" s="412" t="s">
         <v>1191</v>
@@ -45053,7 +44772,7 @@
         <v>912</v>
       </c>
       <c r="E20" s="412" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="F20" s="412" t="s">
         <v>432</v>
@@ -45061,7 +44780,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="413" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="B21" s="412" t="s">
         <v>937</v>
@@ -45073,7 +44792,7 @@
         <v>64</v>
       </c>
       <c r="E21" s="412" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="F21" s="412" t="s">
         <v>432</v>
@@ -45081,10 +44800,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="413" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="B22" s="412" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="C22" s="414">
         <v>3</v>
@@ -45101,10 +44820,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="413" t="s">
+        <v>1409</v>
+      </c>
+      <c r="B23" s="412" t="s">
         <v>1410</v>
-      </c>
-      <c r="B23" s="412" t="s">
-        <v>1411</v>
       </c>
       <c r="C23" s="414">
         <v>3</v>
@@ -45121,10 +44840,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="413" t="s">
+        <v>1411</v>
+      </c>
+      <c r="B24" s="412" t="s">
         <v>1412</v>
-      </c>
-      <c r="B24" s="412" t="s">
-        <v>1413</v>
       </c>
       <c r="C24" s="414">
         <v>3</v>
@@ -45192,17 +44911,17 @@
       </c>
       <c r="E1" s="418"/>
       <c r="F1" s="458" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="410" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="409"/>
       <c r="C2" s="409"/>
       <c r="D2" s="449" t="s">
+        <v>1279</v>
+      </c>
+      <c r="E2" s="449" t="s">
         <v>1280</v>
-      </c>
-      <c r="E2" s="449" t="s">
-        <v>1281</v>
       </c>
       <c r="F2" s="458"/>
     </row>
@@ -45210,7 +44929,7 @@
       <c r="B3" s="409"/>
       <c r="C3" s="409"/>
       <c r="D3" s="449" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="E3" s="449" t="s">
         <v>1136</v>
@@ -45224,10 +44943,10 @@
       <c r="B4" s="464"/>
       <c r="C4" s="464"/>
       <c r="D4" s="449" t="s">
+        <v>1282</v>
+      </c>
+      <c r="E4" s="449" t="s">
         <v>1283</v>
-      </c>
-      <c r="E4" s="449" t="s">
-        <v>1284</v>
       </c>
       <c r="F4" s="449"/>
     </row>
@@ -45236,10 +44955,10 @@
       <c r="B5" s="464"/>
       <c r="C5" s="464"/>
       <c r="D5" s="449" t="s">
+        <v>1284</v>
+      </c>
+      <c r="E5" s="449" t="s">
         <v>1285</v>
-      </c>
-      <c r="E5" s="449" t="s">
-        <v>1286</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="410" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
@@ -45247,7 +44966,7 @@
       <c r="B6" s="464"/>
       <c r="C6" s="464"/>
       <c r="D6" s="449" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="E6" s="449" t="s">
         <v>1230</v>
@@ -45256,15 +44975,15 @@
     </row>
     <row r="7" spans="1:6" s="410" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="464" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="B7" s="464"/>
       <c r="C7" s="464"/>
       <c r="D7" s="449" t="s">
+        <v>1287</v>
+      </c>
+      <c r="E7" s="449" t="s">
         <v>1288</v>
-      </c>
-      <c r="E7" s="449" t="s">
-        <v>1289</v>
       </c>
       <c r="F7" s="449"/>
     </row>
@@ -45273,7 +44992,7 @@
       <c r="B8" s="464"/>
       <c r="C8" s="464"/>
       <c r="D8" s="449" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="E8" s="449" t="s">
         <v>1102</v>
@@ -45284,10 +45003,10 @@
       <c r="B9" s="464"/>
       <c r="C9" s="464"/>
       <c r="D9" s="449" t="s">
+        <v>1290</v>
+      </c>
+      <c r="E9" s="449" t="s">
         <v>1291</v>
-      </c>
-      <c r="E9" s="449" t="s">
-        <v>1292</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="410" customFormat="1" ht="9" x14ac:dyDescent="0.15">
@@ -45295,10 +45014,10 @@
       <c r="B10" s="409"/>
       <c r="C10" s="409"/>
       <c r="D10" s="449" t="s">
+        <v>1292</v>
+      </c>
+      <c r="E10" s="449" t="s">
         <v>1293</v>
-      </c>
-      <c r="E10" s="449" t="s">
-        <v>1294</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="410" customFormat="1" ht="9" x14ac:dyDescent="0.15">
@@ -45329,10 +45048,10 @@
     </row>
     <row r="13" spans="1:6" ht="12" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="413" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B13" s="412" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="C13" s="414">
         <v>3</v>
@@ -45344,15 +45063,15 @@
         <v>914</v>
       </c>
       <c r="F13" s="412" t="s">
-        <v>1439</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="413" t="s">
-        <v>1440</v>
+        <v>1438</v>
       </c>
       <c r="B14" s="412" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="C14" s="414">
         <v>3</v>
@@ -45364,7 +45083,7 @@
         <v>914</v>
       </c>
       <c r="F14" s="412" t="s">
-        <v>1441</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -45381,7 +45100,7 @@
         <v>872</v>
       </c>
       <c r="E15" s="412" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="F15" s="412" t="s">
         <v>14</v>
@@ -45398,7 +45117,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="412" t="s">
-        <v>1442</v>
+        <v>1440</v>
       </c>
       <c r="E16" s="412" t="s">
         <v>933</v>
@@ -45418,7 +45137,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="412" t="s">
-        <v>1442</v>
+        <v>1440</v>
       </c>
       <c r="E17" s="412" t="s">
         <v>1210</v>
@@ -45481,7 +45200,7 @@
         <v>59</v>
       </c>
       <c r="E20" s="412" t="s">
-        <v>1443</v>
+        <v>1441</v>
       </c>
       <c r="F20" s="412" t="s">
         <v>119</v>
@@ -45501,7 +45220,7 @@
         <v>59</v>
       </c>
       <c r="E21" s="412" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="F21" s="412" t="s">
         <v>119</v>
@@ -45521,7 +45240,7 @@
         <v>741</v>
       </c>
       <c r="E22" s="412" t="s">
-        <v>1444</v>
+        <v>1442</v>
       </c>
       <c r="F22" s="412" t="s">
         <v>189</v>
@@ -45558,7 +45277,7 @@
         <v>1</v>
       </c>
       <c r="D24" s="412" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="E24" s="412" t="s">
         <v>919</v>
@@ -45578,7 +45297,7 @@
         <v>1</v>
       </c>
       <c r="D25" s="412" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="E25" s="412" t="s">
         <v>936</v>
@@ -45598,7 +45317,7 @@
         <v>1</v>
       </c>
       <c r="D26" s="412" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="E26" s="412" t="s">
         <v>1034</v>
@@ -45609,7 +45328,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="413" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="B27" s="412" t="s">
         <v>920</v>
@@ -45621,7 +45340,7 @@
         <v>811</v>
       </c>
       <c r="E27" s="412" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="F27" s="412" t="s">
         <v>19</v>
@@ -45629,7 +45348,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="413" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="B28" s="412" t="s">
         <v>920</v>
@@ -45641,7 +45360,7 @@
         <v>811</v>
       </c>
       <c r="E28" s="412" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="F28" s="412" t="s">
         <v>19</v>
@@ -45661,7 +45380,7 @@
         <v>741</v>
       </c>
       <c r="E29" s="412" t="s">
-        <v>1445</v>
+        <v>1443</v>
       </c>
       <c r="F29" s="412" t="s">
         <v>100</v>
@@ -45681,7 +45400,7 @@
         <v>741</v>
       </c>
       <c r="E30" s="412" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="F30" s="412" t="s">
         <v>66</v>
@@ -45701,7 +45420,7 @@
         <v>743</v>
       </c>
       <c r="E31" s="412" t="s">
-        <v>1445</v>
+        <v>1443</v>
       </c>
       <c r="F31" s="412" t="s">
         <v>66</v>
@@ -45721,7 +45440,7 @@
         <v>743</v>
       </c>
       <c r="E32" s="412" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="F32" s="412" t="s">
         <v>100</v>
@@ -45741,7 +45460,7 @@
         <v>811</v>
       </c>
       <c r="E33" s="412" t="s">
-        <v>1446</v>
+        <v>1444</v>
       </c>
       <c r="F33" s="412" t="s">
         <v>100</v>
@@ -45761,7 +45480,7 @@
         <v>811</v>
       </c>
       <c r="E34" s="412" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="F34" s="412" t="s">
         <v>100</v>
@@ -45818,13 +45537,13 @@
         <v>3</v>
       </c>
       <c r="D37" s="412" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="E37" s="412" t="s">
         <v>972</v>
       </c>
       <c r="F37" s="412" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -45844,15 +45563,15 @@
         <v>929</v>
       </c>
       <c r="F38" s="412" t="s">
-        <v>1447</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="413" t="s">
+        <v>1370</v>
+      </c>
+      <c r="B39" s="412" t="s">
         <v>1371</v>
-      </c>
-      <c r="B39" s="412" t="s">
-        <v>1372</v>
       </c>
       <c r="C39" s="414">
         <v>3</v>
@@ -45904,7 +45623,7 @@
         <v>933</v>
       </c>
       <c r="F41" s="412" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -46021,7 +45740,7 @@
         <v>481</v>
       </c>
       <c r="E47" s="412" t="s">
-        <v>1448</v>
+        <v>1446</v>
       </c>
       <c r="F47" s="412" t="s">
         <v>77</v>
@@ -46041,7 +45760,7 @@
         <v>741</v>
       </c>
       <c r="E48" s="412" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="F48" s="412" t="s">
         <v>100</v>
@@ -46081,7 +45800,7 @@
         <v>743</v>
       </c>
       <c r="E50" s="412" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="F50" s="412" t="s">
         <v>100</v>
@@ -46121,7 +45840,7 @@
         <v>741</v>
       </c>
       <c r="E52" s="412" t="s">
-        <v>1450</v>
+        <v>1448</v>
       </c>
       <c r="F52" s="412" t="s">
         <v>100</v>
@@ -46218,7 +45937,7 @@
         <v>2</v>
       </c>
       <c r="D57" s="412" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="E57" s="412" t="s">
         <v>944</v>
@@ -46278,7 +45997,7 @@
         <v>1</v>
       </c>
       <c r="D60" s="412" t="s">
-        <v>1442</v>
+        <v>1440</v>
       </c>
       <c r="E60" s="412" t="s">
         <v>923</v>
@@ -46329,10 +46048,10 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="413" t="s">
+        <v>1372</v>
+      </c>
+      <c r="B63" s="412" t="s">
         <v>1373</v>
-      </c>
-      <c r="B63" s="412" t="s">
-        <v>1374</v>
       </c>
       <c r="C63" s="414">
         <v>1</v>
@@ -46441,7 +46160,7 @@
         <v>481</v>
       </c>
       <c r="E68" s="412" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="F68" s="412" t="s">
         <v>417</v>
@@ -46489,16 +46208,16 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="413" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="B71" s="412" t="s">
-        <v>1453</v>
+        <v>1451</v>
       </c>
       <c r="C71" s="414">
         <v>3</v>
       </c>
       <c r="D71" s="412" t="s">
-        <v>1454</v>
+        <v>1452</v>
       </c>
       <c r="E71" s="412" t="s">
         <v>964</v>
@@ -46549,10 +46268,10 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="413" t="s">
+        <v>1374</v>
+      </c>
+      <c r="B74" s="412" t="s">
         <v>1375</v>
-      </c>
-      <c r="B74" s="412" t="s">
-        <v>1376</v>
       </c>
       <c r="C74" s="414">
         <v>3</v>
@@ -46581,10 +46300,10 @@
         <v>604</v>
       </c>
       <c r="E75" s="412" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="F75" s="412" t="s">
-        <v>1455</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
@@ -46817,7 +46536,7 @@
       </c>
       <c r="E1" s="418"/>
       <c r="F1" s="458" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="410" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
@@ -46957,7 +46676,7 @@
         <v>1001</v>
       </c>
       <c r="B13" s="412" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="C13" s="414">
         <v>3</v>
@@ -46986,7 +46705,7 @@
         <v>533</v>
       </c>
       <c r="E14" s="412" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="F14" s="412" t="s">
         <v>19</v>
@@ -47066,7 +46785,7 @@
         <v>481</v>
       </c>
       <c r="E18" s="412" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="F18" s="412" t="s">
         <v>100</v>
@@ -47086,7 +46805,7 @@
         <v>741</v>
       </c>
       <c r="E19" s="412" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="F19" s="412" t="s">
         <v>100</v>
@@ -47183,7 +46902,7 @@
         <v>1</v>
       </c>
       <c r="D24" s="412" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="E24" s="412" t="s">
         <v>936</v>
@@ -47203,7 +46922,7 @@
         <v>1</v>
       </c>
       <c r="D25" s="412" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="E25" s="412" t="s">
         <v>1034</v>
@@ -47246,7 +46965,7 @@
         <v>159</v>
       </c>
       <c r="E27" s="412" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="F27" s="412" t="s">
         <v>100</v>
@@ -47306,7 +47025,7 @@
         <v>741</v>
       </c>
       <c r="E30" s="412" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="F30" s="412" t="s">
         <v>100</v>
@@ -47326,7 +47045,7 @@
         <v>741</v>
       </c>
       <c r="E31" s="412" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="F31" s="412" t="s">
         <v>100</v>
@@ -47334,7 +47053,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="413" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="B32" s="412" t="s">
         <v>921</v>
@@ -47346,7 +47065,7 @@
         <v>811</v>
       </c>
       <c r="E32" s="412" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="F32" s="412" t="s">
         <v>100</v>
@@ -47354,7 +47073,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="413" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="B33" s="412" t="s">
         <v>921</v>
@@ -47366,7 +47085,7 @@
         <v>811</v>
       </c>
       <c r="E33" s="412" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="F33" s="412" t="s">
         <v>100</v>
@@ -47403,7 +47122,7 @@
         <v>1</v>
       </c>
       <c r="D35" s="412" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="E35" s="412" t="s">
         <v>926</v>
@@ -47423,13 +47142,13 @@
         <v>3</v>
       </c>
       <c r="D36" s="412" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="E36" s="412" t="s">
         <v>1067</v>
       </c>
       <c r="F36" s="412" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -47509,7 +47228,7 @@
         <v>933</v>
       </c>
       <c r="F40" s="412" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -47597,7 +47316,7 @@
         <v>1015</v>
       </c>
       <c r="B45" s="412" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="C45" s="414">
         <v>2</v>
@@ -47606,7 +47325,7 @@
         <v>743</v>
       </c>
       <c r="E45" s="412" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="F45" s="412" t="s">
         <v>100</v>
@@ -47617,7 +47336,7 @@
         <v>1016</v>
       </c>
       <c r="B46" s="412" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="C46" s="414">
         <v>1</v>
@@ -47637,7 +47356,7 @@
         <v>1196</v>
       </c>
       <c r="B47" s="412" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="C47" s="414">
         <v>2</v>
@@ -47657,7 +47376,7 @@
         <v>1198</v>
       </c>
       <c r="B48" s="412" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="C48" s="414">
         <v>1</v>
@@ -47729,7 +47448,7 @@
         <v>944</v>
       </c>
       <c r="F51" s="412" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -47746,7 +47465,7 @@
         <v>184</v>
       </c>
       <c r="E52" s="412" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="F52" s="412" t="s">
         <v>104</v>
@@ -47786,7 +47505,7 @@
         <v>184</v>
       </c>
       <c r="E54" s="412" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="F54" s="412" t="s">
         <v>24</v>
@@ -47834,10 +47553,10 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="413" t="s">
+        <v>1337</v>
+      </c>
+      <c r="B57" s="412" t="s">
         <v>1338</v>
-      </c>
-      <c r="B57" s="412" t="s">
-        <v>1339</v>
       </c>
       <c r="C57" s="414">
         <v>3</v>
@@ -47974,7 +47693,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="413" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="B64" s="412" t="s">
         <v>983</v>
@@ -48054,10 +47773,10 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="413" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B68" s="412" t="s">
         <v>1341</v>
-      </c>
-      <c r="B68" s="412" t="s">
-        <v>1342</v>
       </c>
       <c r="C68" s="414">
         <v>3</v>
@@ -48094,7 +47813,7 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="413" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="B70" s="412" t="s">
         <v>986</v>
@@ -48114,7 +47833,7 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="413" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="B71" s="412" t="s">
         <v>988</v>
@@ -48174,10 +47893,10 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="413" t="s">
+        <v>1367</v>
+      </c>
+      <c r="B74" s="412" t="s">
         <v>1368</v>
-      </c>
-      <c r="B74" s="412" t="s">
-        <v>1369</v>
       </c>
       <c r="C74" s="414">
         <v>3</v>
@@ -48234,7 +47953,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="413" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="B77" s="412" t="s">
         <v>1181</v>

</xml_diff>

<commit_message>
Updated schedule and power lab instructions.
</commit_message>
<xml_diff>
--- a/schedule/semester/schedule.xlsx
+++ b/schedule/semester/schedule.xlsx
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8490" uniqueCount="1505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8523" uniqueCount="1508">
   <si>
     <t>ELECTRICAL AND COMPUTER ENGINEERING</t>
   </si>
@@ -4534,9 +4534,6 @@
     <t>Posted 2/21/2019</t>
   </si>
   <si>
-    <t>Posted 2/20/2019</t>
-  </si>
-  <si>
     <t>SH264/SH260</t>
   </si>
   <si>
@@ -4582,9 +4579,6 @@
     <t>KHC4077</t>
   </si>
   <si>
-    <t>ETC251/ETC252</t>
-  </si>
-  <si>
     <t>ETA309</t>
   </si>
   <si>
@@ -4595,6 +4589,21 @@
   </si>
   <si>
     <t>F 200-340PM</t>
+  </si>
+  <si>
+    <t>Posted 4/23/2019</t>
+  </si>
+  <si>
+    <t>Wang</t>
+  </si>
+  <si>
+    <t>Karuhaka</t>
+  </si>
+  <si>
+    <t>EE3810-06</t>
+  </si>
+  <si>
+    <t>Thorburn</t>
   </si>
 </sst>
 </file>
@@ -28083,7 +28092,7 @@
       <pane xSplit="1" ySplit="12" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="B82" sqref="B82"/>
+      <selection pane="bottomRight" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -28099,7 +28108,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="410" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="407" t="s">
-        <v>1484</v>
+        <v>1503</v>
       </c>
       <c r="B1" s="408"/>
       <c r="C1" s="409"/>
@@ -28260,7 +28269,7 @@
         <v>931</v>
       </c>
       <c r="F13" s="412" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -28273,6 +28282,9 @@
       <c r="C14" s="414">
         <v>1</v>
       </c>
+      <c r="D14" s="412" t="s">
+        <v>1416</v>
+      </c>
       <c r="E14" s="412" t="s">
         <v>1327</v>
       </c>
@@ -28290,6 +28302,9 @@
       <c r="C15" s="414">
         <v>1</v>
       </c>
+      <c r="D15" s="412" t="s">
+        <v>1416</v>
+      </c>
       <c r="E15" s="412" t="s">
         <v>936</v>
       </c>
@@ -28348,7 +28363,7 @@
         <v>481</v>
       </c>
       <c r="E18" s="412" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
       <c r="F18" s="412" t="s">
         <v>100</v>
@@ -28388,7 +28403,7 @@
         <v>481</v>
       </c>
       <c r="E20" s="412" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
       <c r="F20" s="412" t="s">
         <v>100</v>
@@ -28404,8 +28419,11 @@
       <c r="C21" s="414">
         <v>2</v>
       </c>
+      <c r="D21" s="412" t="s">
+        <v>1504</v>
+      </c>
       <c r="E21" s="412" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
       <c r="F21" s="412" t="s">
         <v>100</v>
@@ -28421,8 +28439,11 @@
       <c r="C22" s="414">
         <v>1</v>
       </c>
+      <c r="D22" s="412" t="s">
+        <v>1504</v>
+      </c>
       <c r="E22" s="412" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="F22" s="412" t="s">
         <v>100</v>
@@ -28438,6 +28459,9 @@
       <c r="C23" s="414">
         <v>1</v>
       </c>
+      <c r="D23" s="412" t="s">
+        <v>743</v>
+      </c>
       <c r="E23" s="412" t="s">
         <v>919</v>
       </c>
@@ -28455,6 +28479,9 @@
       <c r="C24" s="414">
         <v>1</v>
       </c>
+      <c r="D24" s="412" t="s">
+        <v>1365</v>
+      </c>
       <c r="E24" s="412" t="s">
         <v>936</v>
       </c>
@@ -28472,6 +28499,9 @@
       <c r="C25" s="414">
         <v>1</v>
       </c>
+      <c r="D25" s="412" t="s">
+        <v>1365</v>
+      </c>
       <c r="E25" s="412" t="s">
         <v>1034</v>
       </c>
@@ -28513,7 +28543,7 @@
         <v>481</v>
       </c>
       <c r="E27" s="412" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
       <c r="F27" s="412" t="s">
         <v>100</v>
@@ -28529,6 +28559,9 @@
       <c r="C28" s="414">
         <v>2</v>
       </c>
+      <c r="D28" s="412" t="s">
+        <v>743</v>
+      </c>
       <c r="E28" s="412" t="s">
         <v>1378</v>
       </c>
@@ -28546,6 +28579,9 @@
       <c r="C29" s="414">
         <v>1</v>
       </c>
+      <c r="D29" s="412" t="s">
+        <v>743</v>
+      </c>
       <c r="E29" s="412" t="s">
         <v>1171</v>
       </c>
@@ -28563,8 +28599,11 @@
       <c r="C30" s="414">
         <v>2</v>
       </c>
+      <c r="D30" s="412" t="s">
+        <v>1504</v>
+      </c>
       <c r="E30" s="412" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="F30" s="412" t="s">
         <v>100</v>
@@ -28580,8 +28619,11 @@
       <c r="C31" s="414">
         <v>1</v>
       </c>
+      <c r="D31" s="412" t="s">
+        <v>1504</v>
+      </c>
       <c r="E31" s="412" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="F31" s="412" t="s">
         <v>100</v>
@@ -28617,6 +28659,9 @@
       <c r="C33" s="414">
         <v>1</v>
       </c>
+      <c r="D33" s="412" t="s">
+        <v>741</v>
+      </c>
       <c r="E33" s="412" t="s">
         <v>926</v>
       </c>
@@ -28626,7 +28671,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="413" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
       <c r="B34" s="412" t="s">
         <v>927</v>
@@ -28643,7 +28688,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="413" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="B35" s="412" t="s">
         <v>927</v>
@@ -28660,7 +28705,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="413" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="B36" s="412" t="s">
         <v>927</v>
@@ -28765,6 +28810,9 @@
       <c r="C41" s="414">
         <v>3</v>
       </c>
+      <c r="D41" s="412" t="s">
+        <v>64</v>
+      </c>
       <c r="E41" s="412" t="s">
         <v>931</v>
       </c>
@@ -28799,6 +28847,9 @@
       <c r="C43" s="414">
         <v>1</v>
       </c>
+      <c r="D43" s="412" t="s">
+        <v>1419</v>
+      </c>
       <c r="E43" s="412" t="s">
         <v>936</v>
       </c>
@@ -28823,7 +28874,7 @@
         <v>942</v>
       </c>
       <c r="F44" s="412" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -28843,7 +28894,7 @@
         <v>938</v>
       </c>
       <c r="F45" s="412" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -28856,6 +28907,9 @@
       <c r="C46" s="414">
         <v>2</v>
       </c>
+      <c r="D46" s="412" t="s">
+        <v>743</v>
+      </c>
       <c r="E46" s="412" t="s">
         <v>1329</v>
       </c>
@@ -28873,6 +28927,9 @@
       <c r="C47" s="414">
         <v>1</v>
       </c>
+      <c r="D47" s="412" t="s">
+        <v>743</v>
+      </c>
       <c r="E47" s="412" t="s">
         <v>1210</v>
       </c>
@@ -28890,8 +28947,11 @@
       <c r="C48" s="414">
         <v>2</v>
       </c>
+      <c r="D48" s="412" t="s">
+        <v>741</v>
+      </c>
       <c r="E48" s="412" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
       <c r="F48" s="412" t="s">
         <v>100</v>
@@ -28907,6 +28967,9 @@
       <c r="C49" s="414">
         <v>1</v>
       </c>
+      <c r="D49" s="412" t="s">
+        <v>741</v>
+      </c>
       <c r="E49" s="412" t="s">
         <v>1034</v>
       </c>
@@ -28924,6 +28987,9 @@
       <c r="C50" s="414">
         <v>1</v>
       </c>
+      <c r="D50" s="412" t="s">
+        <v>741</v>
+      </c>
       <c r="E50" s="412" t="s">
         <v>919</v>
       </c>
@@ -28941,6 +29007,9 @@
       <c r="C51" s="414">
         <v>3</v>
       </c>
+      <c r="D51" s="412" t="s">
+        <v>64</v>
+      </c>
       <c r="E51" s="412" t="s">
         <v>942</v>
       </c>
@@ -28962,10 +29031,10 @@
         <v>184</v>
       </c>
       <c r="E52" s="412" t="s">
+        <v>1497</v>
+      </c>
+      <c r="F52" s="412" t="s">
         <v>1498</v>
-      </c>
-      <c r="F52" s="412" t="s">
-        <v>1499</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -28978,36 +29047,39 @@
       <c r="C53" s="414">
         <v>1</v>
       </c>
+      <c r="D53" s="412" t="s">
+        <v>1505</v>
+      </c>
       <c r="E53" s="412" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
       <c r="F53" s="412" t="s">
-        <v>1500</v>
+        <v>24</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="413" t="s">
-        <v>1161</v>
+        <v>1433</v>
       </c>
       <c r="B54" s="412" t="s">
         <v>943</v>
       </c>
       <c r="C54" s="414">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D54" s="412" t="s">
-        <v>184</v>
+        <v>1505</v>
       </c>
       <c r="E54" s="412" t="s">
-        <v>1498</v>
+        <v>919</v>
       </c>
       <c r="F54" s="412" t="s">
-        <v>1499</v>
+        <v>104</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="413" t="s">
-        <v>1163</v>
+        <v>1506</v>
       </c>
       <c r="B55" s="412" t="s">
         <v>943</v>
@@ -29015,11 +29087,14 @@
       <c r="C55" s="414">
         <v>1</v>
       </c>
+      <c r="D55" s="412" t="s">
+        <v>1440</v>
+      </c>
       <c r="E55" s="412" t="s">
-        <v>1486</v>
+        <v>1207</v>
       </c>
       <c r="F55" s="412" t="s">
-        <v>1500</v>
+        <v>24</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
@@ -29032,6 +29107,9 @@
       <c r="C56" s="414">
         <v>3</v>
       </c>
+      <c r="D56" s="412" t="s">
+        <v>732</v>
+      </c>
       <c r="E56" s="412" t="s">
         <v>946</v>
       </c>
@@ -29049,11 +29127,14 @@
       <c r="C57" s="414">
         <v>3</v>
       </c>
+      <c r="D57" s="412" t="s">
+        <v>414</v>
+      </c>
       <c r="E57" s="412" t="s">
         <v>947</v>
       </c>
       <c r="F57" s="412" t="s">
-        <v>1501</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -29093,7 +29174,7 @@
         <v>972</v>
       </c>
       <c r="F59" s="412" t="s">
-        <v>1502</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -29146,6 +29227,9 @@
       <c r="C62" s="414">
         <v>3</v>
       </c>
+      <c r="D62" s="412" t="s">
+        <v>811</v>
+      </c>
       <c r="E62" s="412" t="s">
         <v>946</v>
       </c>
@@ -29203,6 +29287,9 @@
       <c r="C65" s="414">
         <v>3</v>
       </c>
+      <c r="D65" s="412" t="s">
+        <v>64</v>
+      </c>
       <c r="E65" s="412" t="s">
         <v>962</v>
       </c>
@@ -29220,11 +29307,14 @@
       <c r="C66" s="414">
         <v>3</v>
       </c>
+      <c r="D66" s="412" t="s">
+        <v>1417</v>
+      </c>
       <c r="E66" s="412" t="s">
         <v>972</v>
       </c>
       <c r="F66" s="412" t="s">
-        <v>1503</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -29237,6 +29327,9 @@
       <c r="C67" s="414">
         <v>1</v>
       </c>
+      <c r="D67" s="412" t="s">
+        <v>1419</v>
+      </c>
       <c r="E67" s="412" t="s">
         <v>1207</v>
       </c>
@@ -29254,6 +29347,9 @@
       <c r="C68" s="414">
         <v>3</v>
       </c>
+      <c r="D68" s="412" t="s">
+        <v>64</v>
+      </c>
       <c r="E68" s="412" t="s">
         <v>972</v>
       </c>
@@ -29292,10 +29388,10 @@
         <v>3</v>
       </c>
       <c r="D70" s="412" t="s">
-        <v>604</v>
+        <v>1507</v>
       </c>
       <c r="E70" s="412" t="s">
-        <v>1504</v>
+        <v>1502</v>
       </c>
       <c r="F70" s="412" t="s">
         <v>1225</v>
@@ -29311,6 +29407,9 @@
       <c r="C71" s="414">
         <v>3</v>
       </c>
+      <c r="D71" s="412" t="s">
+        <v>166</v>
+      </c>
       <c r="E71" s="412" t="s">
         <v>958</v>
       </c>
@@ -29328,6 +29427,9 @@
       <c r="C72" s="414">
         <v>3</v>
       </c>
+      <c r="D72" s="412" t="s">
+        <v>414</v>
+      </c>
       <c r="E72" s="412" t="s">
         <v>972</v>
       </c>
@@ -29345,6 +29447,9 @@
       <c r="C73" s="414">
         <v>3</v>
       </c>
+      <c r="D73" s="412" t="s">
+        <v>414</v>
+      </c>
       <c r="E73" s="412" t="s">
         <v>964</v>
       </c>
@@ -29403,7 +29508,7 @@
         <v>3</v>
       </c>
       <c r="D76" s="412" t="s">
-        <v>59</v>
+        <v>811</v>
       </c>
       <c r="E76" s="412" t="s">
         <v>947</v>
@@ -29421,6 +29526,9 @@
       </c>
       <c r="C77" s="414">
         <v>3</v>
+      </c>
+      <c r="D77" s="412" t="s">
+        <v>166</v>
       </c>
       <c r="E77" s="412" t="s">
         <v>969</v>

</xml_diff>

<commit_message>
Fall 2019 Schedule update
</commit_message>
<xml_diff>
--- a/schedule/semester/schedule.xlsx
+++ b/schedule/semester/schedule.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5250" yWindow="75" windowWidth="16320" windowHeight="12375" tabRatio="734" activeTab="3"/>
+    <workbookView xWindow="5250" yWindow="75" windowWidth="16320" windowHeight="12375" tabRatio="734" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="sum20" sheetId="83" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8518" uniqueCount="1505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8519" uniqueCount="1506">
   <si>
     <t>ELECTRICAL AND COMPUTER ENGINEERING</t>
   </si>
@@ -4591,10 +4591,13 @@
     <t>Thorburn</t>
   </si>
   <si>
-    <t>Posted 5/6/2019</t>
-  </si>
-  <si>
     <t>Posted 5/20/2019</t>
+  </si>
+  <si>
+    <t>SH358B</t>
+  </si>
+  <si>
+    <t>Posted 6/5/2019</t>
   </si>
 </sst>
 </file>
@@ -28079,11 +28082,11 @@
   </sheetPr>
   <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" ySplit="12" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="I16" sqref="I16"/>
+      <selection pane="bottomRight" activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -28099,7 +28102,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="410" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="407" t="s">
-        <v>1503</v>
+        <v>1505</v>
       </c>
       <c r="B1" s="408"/>
       <c r="C1" s="409"/>
@@ -28768,7 +28771,7 @@
         <v>938</v>
       </c>
       <c r="F39" s="412" t="s">
-        <v>1394</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -28820,6 +28823,9 @@
       </c>
       <c r="C42" s="414">
         <v>3</v>
+      </c>
+      <c r="D42" s="412" t="s">
+        <v>64</v>
       </c>
       <c r="E42" s="412" t="s">
         <v>964</v>
@@ -37656,7 +37662,7 @@
   </sheetPr>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" ySplit="12" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
@@ -37676,7 +37682,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="410" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="407" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="B1" s="408"/>
       <c r="C1" s="409"/>

</xml_diff>

<commit_message>
Added Spring 2020 Schedule
</commit_message>
<xml_diff>
--- a/schedule/semester/schedule.xlsx
+++ b/schedule/semester/schedule.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5250" yWindow="75" windowWidth="16320" windowHeight="12375" tabRatio="734" activeTab="2"/>
+    <workbookView xWindow="5250" yWindow="75" windowWidth="16320" windowHeight="12375" tabRatio="734" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="sum20" sheetId="83" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8493" uniqueCount="1502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8804" uniqueCount="1529">
   <si>
     <t>ELECTRICAL AND COMPUTER ENGINEERING</t>
   </si>
@@ -4586,6 +4586,87 @@
   </si>
   <si>
     <t>Posted 8/26/2019</t>
+  </si>
+  <si>
+    <t>TR 800-850AM</t>
+  </si>
+  <si>
+    <t>TR 905-1020AM</t>
+  </si>
+  <si>
+    <t>WF140-230PM</t>
+  </si>
+  <si>
+    <t>WF 245-400PM</t>
+  </si>
+  <si>
+    <t>M 1055AM-125PM</t>
+  </si>
+  <si>
+    <t>W 1055AM-125PM</t>
+  </si>
+  <si>
+    <t>MW 905-1020AM</t>
+  </si>
+  <si>
+    <t>WF 430-520PM</t>
+  </si>
+  <si>
+    <t>WF 535-650PM</t>
+  </si>
+  <si>
+    <t>T 150-420PM</t>
+  </si>
+  <si>
+    <t>KHC4077</t>
+  </si>
+  <si>
+    <t>MW 430-545pm</t>
+  </si>
+  <si>
+    <t>TR 1050AM-1140AM</t>
+  </si>
+  <si>
+    <t>TR 1155AM-110PM</t>
+  </si>
+  <si>
+    <t>TR 600-650PM</t>
+  </si>
+  <si>
+    <t>TR 705-820PM</t>
+  </si>
+  <si>
+    <t>MW 1205-120PM</t>
+  </si>
+  <si>
+    <t>TR 500-550PM</t>
+  </si>
+  <si>
+    <t>WF 725-840PM</t>
+  </si>
+  <si>
+    <t>TR 140-230PM</t>
+  </si>
+  <si>
+    <t>TR 245-400PM</t>
+  </si>
+  <si>
+    <t>EE4630</t>
+  </si>
+  <si>
+    <t>Machine Learning Principles and Applications</t>
+  </si>
+  <si>
+    <t>Vincent, P.</t>
+  </si>
+  <si>
+    <t>KHLH2</t>
+  </si>
+  <si>
+    <t>Linear Sys Analysis</t>
+  </si>
+  <si>
+    <t>Posted  10/1/2019</t>
   </si>
 </sst>
 </file>
@@ -18981,13 +19062,13 @@
   <sheetPr codeName="Sheet41">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" ySplit="12" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="B28" sqref="B28"/>
+      <selection pane="bottomRight" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -19003,7 +19084,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="410" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="407" t="s">
-        <v>1113</v>
+        <v>1528</v>
       </c>
       <c r="B1" s="408"/>
       <c r="C1" s="409"/>
@@ -19142,7 +19223,1254 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="12" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:6" ht="12" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="413" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B13" s="412" t="s">
+        <v>1364</v>
+      </c>
+      <c r="C13" s="414">
+        <v>3</v>
+      </c>
+      <c r="D13" s="412" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="412" t="s">
+        <v>914</v>
+      </c>
+      <c r="F13" s="412" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="413" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B14" s="412" t="s">
+        <v>915</v>
+      </c>
+      <c r="C14" s="414">
+        <v>1</v>
+      </c>
+      <c r="D14" s="412" t="s">
+        <v>1416</v>
+      </c>
+      <c r="E14" s="412" t="s">
+        <v>933</v>
+      </c>
+      <c r="F14" s="412" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="413" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B15" s="412" t="s">
+        <v>915</v>
+      </c>
+      <c r="C15" s="414">
+        <v>1</v>
+      </c>
+      <c r="D15" s="412" t="s">
+        <v>1416</v>
+      </c>
+      <c r="E15" s="412" t="s">
+        <v>1210</v>
+      </c>
+      <c r="F15" s="412" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="413" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B16" s="412" t="s">
+        <v>915</v>
+      </c>
+      <c r="C16" s="414">
+        <v>1</v>
+      </c>
+      <c r="E16" s="412" t="s">
+        <v>926</v>
+      </c>
+      <c r="F16" s="412" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="413" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B17" s="412" t="s">
+        <v>917</v>
+      </c>
+      <c r="C17" s="414">
+        <v>2</v>
+      </c>
+      <c r="D17" s="412" t="s">
+        <v>1491</v>
+      </c>
+      <c r="E17" s="412" t="s">
+        <v>1502</v>
+      </c>
+      <c r="F17" s="412" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="413" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B18" s="412" t="s">
+        <v>917</v>
+      </c>
+      <c r="C18" s="414">
+        <v>1</v>
+      </c>
+      <c r="D18" s="412" t="s">
+        <v>1491</v>
+      </c>
+      <c r="E18" s="412" t="s">
+        <v>1503</v>
+      </c>
+      <c r="F18" s="412" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="413" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B19" s="412" t="s">
+        <v>917</v>
+      </c>
+      <c r="C19" s="414">
+        <v>2</v>
+      </c>
+      <c r="D19" s="412" t="s">
+        <v>481</v>
+      </c>
+      <c r="E19" s="412" t="s">
+        <v>1504</v>
+      </c>
+      <c r="F19" s="412" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="413" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B20" s="412" t="s">
+        <v>917</v>
+      </c>
+      <c r="C20" s="414">
+        <v>1</v>
+      </c>
+      <c r="D20" s="412" t="s">
+        <v>481</v>
+      </c>
+      <c r="E20" s="412" t="s">
+        <v>1505</v>
+      </c>
+      <c r="F20" s="412" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="413" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B21" s="412" t="s">
+        <v>920</v>
+      </c>
+      <c r="C21" s="414">
+        <v>1</v>
+      </c>
+      <c r="D21" s="412" t="s">
+        <v>1365</v>
+      </c>
+      <c r="E21" s="412" t="s">
+        <v>936</v>
+      </c>
+      <c r="F21" s="412" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="413" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B22" s="412" t="s">
+        <v>920</v>
+      </c>
+      <c r="C22" s="414">
+        <v>1</v>
+      </c>
+      <c r="D22" s="412" t="s">
+        <v>811</v>
+      </c>
+      <c r="E22" s="412" t="s">
+        <v>1506</v>
+      </c>
+      <c r="F22" s="412" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="413" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B23" s="412" t="s">
+        <v>920</v>
+      </c>
+      <c r="C23" s="414">
+        <v>1</v>
+      </c>
+      <c r="D23" s="412" t="s">
+        <v>811</v>
+      </c>
+      <c r="E23" s="412" t="s">
+        <v>1507</v>
+      </c>
+      <c r="F23" s="412" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="413" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B24" s="412" t="s">
+        <v>921</v>
+      </c>
+      <c r="C24" s="414">
+        <v>2</v>
+      </c>
+      <c r="D24" s="412" t="s">
+        <v>159</v>
+      </c>
+      <c r="E24" s="412" t="s">
+        <v>1441</v>
+      </c>
+      <c r="F24" s="412" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="413" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B25" s="412" t="s">
+        <v>921</v>
+      </c>
+      <c r="C25" s="414">
+        <v>1</v>
+      </c>
+      <c r="D25" s="412" t="s">
+        <v>159</v>
+      </c>
+      <c r="E25" s="412" t="s">
+        <v>1508</v>
+      </c>
+      <c r="F25" s="412" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="413" t="s">
+        <v>1168</v>
+      </c>
+      <c r="B26" s="412" t="s">
+        <v>921</v>
+      </c>
+      <c r="C26" s="414">
+        <v>2</v>
+      </c>
+      <c r="D26" s="412" t="s">
+        <v>481</v>
+      </c>
+      <c r="E26" s="412" t="s">
+        <v>1509</v>
+      </c>
+      <c r="F26" s="412" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="413" t="s">
+        <v>1170</v>
+      </c>
+      <c r="B27" s="412" t="s">
+        <v>921</v>
+      </c>
+      <c r="C27" s="414">
+        <v>1</v>
+      </c>
+      <c r="D27" s="412" t="s">
+        <v>481</v>
+      </c>
+      <c r="E27" s="412" t="s">
+        <v>1510</v>
+      </c>
+      <c r="F27" s="412" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="413" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B28" s="412" t="s">
+        <v>1191</v>
+      </c>
+      <c r="C28" s="414">
+        <v>3</v>
+      </c>
+      <c r="D28" s="412" t="s">
+        <v>912</v>
+      </c>
+      <c r="E28" s="412" t="s">
+        <v>924</v>
+      </c>
+      <c r="F28" s="412" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="413" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B29" s="412" t="s">
+        <v>925</v>
+      </c>
+      <c r="C29" s="414">
+        <v>1</v>
+      </c>
+      <c r="D29" s="412" t="s">
+        <v>741</v>
+      </c>
+      <c r="E29" s="412" t="s">
+        <v>1511</v>
+      </c>
+      <c r="F29" s="412" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="413" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B30" s="412" t="s">
+        <v>1179</v>
+      </c>
+      <c r="C30" s="414">
+        <v>3</v>
+      </c>
+      <c r="D30" s="412" t="s">
+        <v>64</v>
+      </c>
+      <c r="E30" s="412" t="s">
+        <v>929</v>
+      </c>
+      <c r="F30" s="412" t="s">
+        <v>1512</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="413" t="s">
+        <v>1370</v>
+      </c>
+      <c r="B31" s="412" t="s">
+        <v>1371</v>
+      </c>
+      <c r="C31" s="414">
+        <v>3</v>
+      </c>
+      <c r="D31" s="412" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31" s="412" t="s">
+        <v>914</v>
+      </c>
+      <c r="F31" s="412" t="s">
+        <v>1496</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="413" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B32" s="412" t="s">
+        <v>930</v>
+      </c>
+      <c r="C32" s="414">
+        <v>3</v>
+      </c>
+      <c r="D32" s="412" t="s">
+        <v>34</v>
+      </c>
+      <c r="E32" s="412" t="s">
+        <v>931</v>
+      </c>
+      <c r="F32" s="412" t="s">
+        <v>1496</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="413" t="s">
+        <v>1213</v>
+      </c>
+      <c r="B33" s="412" t="s">
+        <v>934</v>
+      </c>
+      <c r="C33" s="414">
+        <v>3</v>
+      </c>
+      <c r="D33" s="412" t="s">
+        <v>64</v>
+      </c>
+      <c r="E33" s="412" t="s">
+        <v>931</v>
+      </c>
+      <c r="F33" s="412" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="413" t="s">
+        <v>1214</v>
+      </c>
+      <c r="B34" s="412" t="s">
+        <v>934</v>
+      </c>
+      <c r="C34" s="414">
+        <v>3</v>
+      </c>
+      <c r="D34" s="412" t="s">
+        <v>467</v>
+      </c>
+      <c r="E34" s="412" t="s">
+        <v>1513</v>
+      </c>
+      <c r="F34" s="412" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="413" t="s">
+        <v>1418</v>
+      </c>
+      <c r="B35" s="412" t="s">
+        <v>935</v>
+      </c>
+      <c r="C35" s="414">
+        <v>1</v>
+      </c>
+      <c r="D35" s="412" t="s">
+        <v>1419</v>
+      </c>
+      <c r="E35" s="412" t="s">
+        <v>936</v>
+      </c>
+      <c r="F35" s="412" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="413" t="s">
+        <v>1420</v>
+      </c>
+      <c r="B36" s="412" t="s">
+        <v>935</v>
+      </c>
+      <c r="C36" s="414">
+        <v>1</v>
+      </c>
+      <c r="D36" s="412" t="s">
+        <v>1419</v>
+      </c>
+      <c r="E36" s="412" t="s">
+        <v>933</v>
+      </c>
+      <c r="F36" s="412" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="413" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B37" s="412" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C37" s="414">
+        <v>3</v>
+      </c>
+      <c r="D37" s="412" t="s">
+        <v>1421</v>
+      </c>
+      <c r="E37" s="412" t="s">
+        <v>942</v>
+      </c>
+      <c r="F37" s="412" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="413" t="s">
+        <v>1156</v>
+      </c>
+      <c r="B38" s="412" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C38" s="414">
+        <v>3</v>
+      </c>
+      <c r="D38" s="412" t="s">
+        <v>1421</v>
+      </c>
+      <c r="E38" s="412" t="s">
+        <v>938</v>
+      </c>
+      <c r="F38" s="412" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="413" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B39" s="412" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C39" s="414">
+        <v>2</v>
+      </c>
+      <c r="D39" s="412" t="s">
+        <v>1491</v>
+      </c>
+      <c r="E39" s="412" t="s">
+        <v>1514</v>
+      </c>
+      <c r="F39" s="412" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="413" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B40" s="412" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C40" s="414">
+        <v>1</v>
+      </c>
+      <c r="D40" s="412" t="s">
+        <v>1491</v>
+      </c>
+      <c r="E40" s="412" t="s">
+        <v>1515</v>
+      </c>
+      <c r="F40" s="412" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="413" t="s">
+        <v>1196</v>
+      </c>
+      <c r="B41" s="412" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C41" s="414">
+        <v>2</v>
+      </c>
+      <c r="D41" s="412" t="s">
+        <v>743</v>
+      </c>
+      <c r="E41" s="412" t="s">
+        <v>1516</v>
+      </c>
+      <c r="F41" s="412" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="413" t="s">
+        <v>1198</v>
+      </c>
+      <c r="B42" s="412" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C42" s="414">
+        <v>1</v>
+      </c>
+      <c r="D42" s="412" t="s">
+        <v>743</v>
+      </c>
+      <c r="E42" s="412" t="s">
+        <v>1517</v>
+      </c>
+      <c r="F42" s="412" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="413" t="s">
+        <v>1199</v>
+      </c>
+      <c r="B43" s="412" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C43" s="414">
+        <v>2</v>
+      </c>
+      <c r="D43" s="412" t="s">
+        <v>743</v>
+      </c>
+      <c r="E43" s="412" t="s">
+        <v>1062</v>
+      </c>
+      <c r="F43" s="412" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="413" t="s">
+        <v>1201</v>
+      </c>
+      <c r="B44" s="412" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C44" s="414">
+        <v>1</v>
+      </c>
+      <c r="D44" s="412" t="s">
+        <v>743</v>
+      </c>
+      <c r="E44" s="412" t="s">
+        <v>1518</v>
+      </c>
+      <c r="F44" s="412" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="413" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B45" s="412" t="s">
+        <v>1202</v>
+      </c>
+      <c r="C45" s="414">
+        <v>3</v>
+      </c>
+      <c r="D45" s="412" t="s">
+        <v>34</v>
+      </c>
+      <c r="E45" s="412" t="s">
+        <v>929</v>
+      </c>
+      <c r="F45" s="412" t="s">
+        <v>1496</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="413" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B46" s="412" t="s">
+        <v>937</v>
+      </c>
+      <c r="C46" s="414">
+        <v>3</v>
+      </c>
+      <c r="D46" s="412" t="s">
+        <v>34</v>
+      </c>
+      <c r="E46" s="412" t="s">
+        <v>938</v>
+      </c>
+      <c r="F46" s="412" t="s">
+        <v>1496</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="413" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B47" s="412" t="s">
+        <v>941</v>
+      </c>
+      <c r="C47" s="414">
+        <v>3</v>
+      </c>
+      <c r="D47" s="412" t="s">
+        <v>64</v>
+      </c>
+      <c r="E47" s="412" t="s">
+        <v>942</v>
+      </c>
+      <c r="F47" s="412" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="413" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B48" s="412" t="s">
+        <v>943</v>
+      </c>
+      <c r="C48" s="414">
+        <v>2</v>
+      </c>
+      <c r="D48" s="412" t="s">
+        <v>741</v>
+      </c>
+      <c r="E48" s="412" t="s">
+        <v>1519</v>
+      </c>
+      <c r="F48" s="412" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="413" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B49" s="412" t="s">
+        <v>943</v>
+      </c>
+      <c r="C49" s="414">
+        <v>1</v>
+      </c>
+      <c r="D49" s="412" t="s">
+        <v>741</v>
+      </c>
+      <c r="E49" s="412" t="s">
+        <v>919</v>
+      </c>
+      <c r="F49" s="412" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="413" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B50" s="412" t="s">
+        <v>943</v>
+      </c>
+      <c r="C50" s="414">
+        <v>1</v>
+      </c>
+      <c r="D50" s="412" t="s">
+        <v>741</v>
+      </c>
+      <c r="E50" s="412" t="s">
+        <v>1484</v>
+      </c>
+      <c r="F50" s="412" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="413" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B51" s="412" t="s">
+        <v>943</v>
+      </c>
+      <c r="C51" s="414">
+        <v>1</v>
+      </c>
+      <c r="D51" s="412" t="s">
+        <v>741</v>
+      </c>
+      <c r="E51" s="412" t="s">
+        <v>1207</v>
+      </c>
+      <c r="F51" s="412" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="413" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B52" s="412" t="s">
+        <v>945</v>
+      </c>
+      <c r="C52" s="414">
+        <v>3</v>
+      </c>
+      <c r="D52" s="412" t="s">
+        <v>732</v>
+      </c>
+      <c r="E52" s="412" t="s">
+        <v>946</v>
+      </c>
+      <c r="F52" s="412" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="413" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B53" s="412" t="s">
+        <v>948</v>
+      </c>
+      <c r="C53" s="414">
+        <v>3</v>
+      </c>
+      <c r="D53" s="412" t="s">
+        <v>414</v>
+      </c>
+      <c r="E53" s="412" t="s">
+        <v>947</v>
+      </c>
+      <c r="F53" s="412" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="413" t="s">
+        <v>1372</v>
+      </c>
+      <c r="B54" s="412" t="s">
+        <v>1373</v>
+      </c>
+      <c r="C54" s="414">
+        <v>1</v>
+      </c>
+      <c r="D54" s="412" t="s">
+        <v>1417</v>
+      </c>
+      <c r="E54" s="412" t="s">
+        <v>1210</v>
+      </c>
+      <c r="F54" s="412" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="413" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B55" s="412" t="s">
+        <v>949</v>
+      </c>
+      <c r="C55" s="414">
+        <v>3</v>
+      </c>
+      <c r="E55" s="412" t="s">
+        <v>964</v>
+      </c>
+      <c r="F55" s="412" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="413" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B56" s="412" t="s">
+        <v>951</v>
+      </c>
+      <c r="C56" s="414">
+        <v>3</v>
+      </c>
+      <c r="D56" s="412" t="s">
+        <v>476</v>
+      </c>
+      <c r="E56" s="412" t="s">
+        <v>928</v>
+      </c>
+      <c r="F56" s="412" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="413" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B57" s="412" t="s">
+        <v>952</v>
+      </c>
+      <c r="C57" s="414">
+        <v>3</v>
+      </c>
+      <c r="D57" s="412" t="s">
+        <v>1218</v>
+      </c>
+      <c r="E57" s="412" t="s">
+        <v>924</v>
+      </c>
+      <c r="F57" s="412" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="413" t="s">
+        <v>1077</v>
+      </c>
+      <c r="B58" s="412" t="s">
+        <v>955</v>
+      </c>
+      <c r="C58" s="414">
+        <v>3</v>
+      </c>
+      <c r="D58" s="412" t="s">
+        <v>1218</v>
+      </c>
+      <c r="E58" s="412" t="s">
+        <v>1173</v>
+      </c>
+      <c r="F58" s="412" t="s">
+        <v>1497</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="413" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B59" s="412" t="s">
+        <v>957</v>
+      </c>
+      <c r="C59" s="414">
+        <v>3</v>
+      </c>
+      <c r="D59" s="412" t="s">
+        <v>481</v>
+      </c>
+      <c r="E59" s="412" t="s">
+        <v>1520</v>
+      </c>
+      <c r="F59" s="412" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="413" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B60" s="412" t="s">
+        <v>983</v>
+      </c>
+      <c r="C60" s="414">
+        <v>3</v>
+      </c>
+      <c r="E60" s="412" t="s">
+        <v>946</v>
+      </c>
+      <c r="F60" s="412" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="413" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B61" s="412" t="s">
+        <v>959</v>
+      </c>
+      <c r="C61" s="414">
+        <v>2</v>
+      </c>
+      <c r="D61" s="412" t="s">
+        <v>743</v>
+      </c>
+      <c r="E61" s="412" t="s">
+        <v>1521</v>
+      </c>
+      <c r="F61" s="412" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="413" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B62" s="412" t="s">
+        <v>959</v>
+      </c>
+      <c r="C62" s="414">
+        <v>1</v>
+      </c>
+      <c r="D62" s="412" t="s">
+        <v>743</v>
+      </c>
+      <c r="E62" s="412" t="s">
+        <v>1522</v>
+      </c>
+      <c r="F62" s="412" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="413" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B63" s="412" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C63" s="414">
+        <v>3</v>
+      </c>
+      <c r="D63" s="412" t="s">
+        <v>64</v>
+      </c>
+      <c r="E63" s="412" t="s">
+        <v>962</v>
+      </c>
+      <c r="F63" s="412" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="413" t="s">
+        <v>1523</v>
+      </c>
+      <c r="B64" s="412" t="s">
+        <v>1524</v>
+      </c>
+      <c r="C64" s="414">
+        <v>3</v>
+      </c>
+      <c r="D64" s="412" t="s">
+        <v>414</v>
+      </c>
+      <c r="E64" s="412" t="s">
+        <v>950</v>
+      </c>
+      <c r="F64" s="412" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="413" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B65" s="412" t="s">
+        <v>963</v>
+      </c>
+      <c r="C65" s="414">
+        <v>1</v>
+      </c>
+      <c r="D65" s="412" t="s">
+        <v>1419</v>
+      </c>
+      <c r="E65" s="412" t="s">
+        <v>1207</v>
+      </c>
+      <c r="F65" s="412" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="413" t="s">
+        <v>1374</v>
+      </c>
+      <c r="B66" s="412" t="s">
+        <v>1375</v>
+      </c>
+      <c r="C66" s="414">
+        <v>3</v>
+      </c>
+      <c r="D66" s="412" t="s">
+        <v>1525</v>
+      </c>
+      <c r="E66" s="412" t="s">
+        <v>972</v>
+      </c>
+      <c r="F66" s="412" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="413" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B67" s="412" t="s">
+        <v>965</v>
+      </c>
+      <c r="C67" s="414">
+        <v>3</v>
+      </c>
+      <c r="D67" s="412" t="s">
+        <v>1494</v>
+      </c>
+      <c r="E67" s="412" t="s">
+        <v>1490</v>
+      </c>
+      <c r="F67" s="412" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="413" t="s">
+        <v>1084</v>
+      </c>
+      <c r="B68" s="412" t="s">
+        <v>968</v>
+      </c>
+      <c r="C68" s="414">
+        <v>3</v>
+      </c>
+      <c r="E68" s="412" t="s">
+        <v>969</v>
+      </c>
+      <c r="F68" s="412" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="413" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B69" s="412" t="s">
+        <v>970</v>
+      </c>
+      <c r="C69" s="414">
+        <v>3</v>
+      </c>
+      <c r="D69" s="412" t="s">
+        <v>166</v>
+      </c>
+      <c r="E69" s="412" t="s">
+        <v>953</v>
+      </c>
+      <c r="F69" s="412" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="413" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B70" s="412" t="s">
+        <v>971</v>
+      </c>
+      <c r="C70" s="414">
+        <v>3</v>
+      </c>
+      <c r="D70" s="412" t="s">
+        <v>414</v>
+      </c>
+      <c r="E70" s="412" t="s">
+        <v>972</v>
+      </c>
+      <c r="F70" s="412" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="413" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B71" s="412" t="s">
+        <v>990</v>
+      </c>
+      <c r="C71" s="414">
+        <v>3</v>
+      </c>
+      <c r="D71" s="412" t="s">
+        <v>45</v>
+      </c>
+      <c r="E71" s="412" t="s">
+        <v>964</v>
+      </c>
+      <c r="F71" s="412" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="413" t="s">
+        <v>1087</v>
+      </c>
+      <c r="B72" s="412" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C72" s="414">
+        <v>3</v>
+      </c>
+      <c r="D72" s="412" t="s">
+        <v>754</v>
+      </c>
+      <c r="E72" s="412" t="s">
+        <v>924</v>
+      </c>
+      <c r="F72" s="412" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="413" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B73" s="412" t="s">
+        <v>973</v>
+      </c>
+      <c r="C73" s="414">
+        <v>3</v>
+      </c>
+      <c r="D73" s="412" t="s">
+        <v>607</v>
+      </c>
+      <c r="E73" s="412" t="s">
+        <v>1067</v>
+      </c>
+      <c r="F73" s="412" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="413" t="s">
+        <v>1090</v>
+      </c>
+      <c r="B74" s="412" t="s">
+        <v>1188</v>
+      </c>
+      <c r="C74" s="414">
+        <v>3</v>
+      </c>
+      <c r="D74" s="412" t="s">
+        <v>811</v>
+      </c>
+      <c r="E74" s="412" t="s">
+        <v>947</v>
+      </c>
+      <c r="F74" s="412" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="413" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B75" s="412" t="s">
+        <v>1527</v>
+      </c>
+      <c r="C75" s="414">
+        <v>3</v>
+      </c>
+      <c r="D75" s="412" t="s">
+        <v>166</v>
+      </c>
+      <c r="E75" s="412" t="s">
+        <v>958</v>
+      </c>
+      <c r="F75" s="412" t="s">
+        <v>228</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A4:C6"/>
@@ -28070,7 +29398,7 @@
   </sheetPr>
   <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" ySplit="12" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>

</xml_diff>